<commit_message>
Anova motivation analysis using a measurement instrument of RSM
</commit_message>
<xml_diff>
--- a/exp2/case01/report/motivation/interest-enjoyment/MeasurementModel.xlsx
+++ b/exp2/case01/report/motivation/interest-enjoyment/MeasurementModel.xlsx
@@ -2312,10 +2312,10 @@
         <v>4.0</v>
       </c>
       <c r="B6" t="n" s="32">
-        <v>691.0115778615361</v>
+        <v>691.011577861536</v>
       </c>
       <c r="C6" t="n" s="33">
-        <v>-345.50578893076806</v>
+        <v>-345.505788930768</v>
       </c>
       <c r="D6" t="n" s="34">
         <v>56.0</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="11">
       <c r="A11" t="n" s="56">
-        <v>0.18382750892487643</v>
+        <v>0.18382750892487698</v>
       </c>
       <c r="B11" t="n" s="57">
-        <v>0.3202448986074695</v>
+        <v>0.32024489860746974</v>
       </c>
       <c r="C11" t="n" s="58">
-        <v>0.11838795895159568</v>
+        <v>0.11838795895159522</v>
       </c>
     </row>
     <row r="12">
@@ -2395,7 +2395,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n" s="77">
-        <v>401.22500919061474</v>
+        <v>401.2250091906144</v>
       </c>
       <c r="B16" t="n" s="78">
         <v>6.0</v>
@@ -2432,13 +2432,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n" s="98">
-        <v>15.081334650665518</v>
+        <v>15.081334650665399</v>
       </c>
       <c r="B21" t="n" s="99">
-        <v>0.10834929265378065</v>
+        <v>0.10834929265378099</v>
       </c>
       <c r="C21" t="n" s="100">
-        <v>0.1317667457549639</v>
+        <v>0.13176674575496422</v>
       </c>
     </row>
     <row r="22">
@@ -2499,10 +2499,10 @@
         <v>49.0</v>
       </c>
       <c r="F26" t="n" s="124">
-        <v>28.517863376251356</v>
+        <v>28.51786337625131</v>
       </c>
       <c r="G26" t="n" s="125">
-        <v>0.9915237821250712</v>
+        <v>0.9915237821250713</v>
       </c>
       <c r="H26" t="n" s="126">
         <v>1.0</v>
@@ -2525,10 +2525,10 @@
         <v>49.0</v>
       </c>
       <c r="F27" t="n" s="124">
-        <v>30.746755743442716</v>
+        <v>30.74675574344263</v>
       </c>
       <c r="G27" t="n" s="125">
-        <v>0.98081597840602</v>
+        <v>0.9808159784060205</v>
       </c>
       <c r="H27" t="n" s="126">
         <v>1.0</v>
@@ -2551,7 +2551,7 @@
         <v>49.0</v>
       </c>
       <c r="F28" t="n" s="124">
-        <v>401.22500919061474</v>
+        <v>401.2250091906144</v>
       </c>
       <c r="G28" t="n" s="125">
         <v>0.0</v>
@@ -2577,10 +2577,10 @@
         <v>49.0</v>
       </c>
       <c r="F29" t="n" s="124">
-        <v>29.605416996562465</v>
+        <v>29.605416996562457</v>
       </c>
       <c r="G29" t="n" s="125">
-        <v>0.98716178504944</v>
+        <v>0.9871617850494399</v>
       </c>
       <c r="H29" t="n" s="126">
         <v>1.0</v>
@@ -2603,7 +2603,7 @@
         <v>49.0</v>
       </c>
       <c r="F30" t="n" s="124">
-        <v>252.10965773795832</v>
+        <v>252.10965773795823</v>
       </c>
       <c r="G30" t="n" s="125">
         <v>0.0</v>
@@ -2629,7 +2629,7 @@
         <v>49.0</v>
       </c>
       <c r="F31" t="n" s="124">
-        <v>227.43068289925918</v>
+        <v>227.4306828992593</v>
       </c>
       <c r="G31" t="n" s="125">
         <v>0.0</v>
@@ -2669,27 +2669,27 @@
     </row>
     <row r="36">
       <c r="A36" t="n" s="145">
-        <v>-1.127478008663923</v>
+        <v>-1.1274780086639238</v>
       </c>
       <c r="B36" t="n" s="146">
-        <v>0.17438621218697303</v>
+        <v>0.17438621218697214</v>
       </c>
       <c r="C36" t="n" s="147">
-        <v>0.6682151469316651</v>
+        <v>0.6682151469316642</v>
       </c>
       <c r="D36" t="n" s="148">
-        <v>0.9275565670613153</v>
+        <v>0.9275565670613126</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n" s="145">
-        <v>0.4899230181024885</v>
+        <v>0.4899230181024876</v>
       </c>
       <c r="B37" t="n" s="146">
-        <v>-0.2276859391685102</v>
+        <v>-0.22768593916850932</v>
       </c>
       <c r="C37" t="n" s="147">
-        <v>0.2933496827570403</v>
+        <v>0.2933496827570412</v>
       </c>
       <c r="D37" t="n" s="148">
         <v>-0.4580200728975514</v>
@@ -2700,41 +2700,41 @@
         <v>0.44085823824134085</v>
       </c>
       <c r="B38" t="n" s="146">
-        <v>-0.16521922158592073</v>
+        <v>-0.16521922158591984</v>
       </c>
       <c r="C38" t="n" s="147">
-        <v>0.25227000447750036</v>
+        <v>0.2522700044774986</v>
       </c>
       <c r="D38" t="n" s="148">
-        <v>0.49326618176885795</v>
+        <v>0.49326618176885706</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n" s="145">
-        <v>1.081930474551065</v>
+        <v>1.081930474551064</v>
       </c>
       <c r="B39" t="n" s="146">
         <v>0.3629693801357776</v>
       </c>
       <c r="C39" t="n" s="147">
-        <v>-0.12266641253456623</v>
+        <v>-0.12266641253456445</v>
       </c>
       <c r="D39" t="n" s="148">
-        <v>-0.8635595535144844</v>
+        <v>-0.8635595535144853</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n" s="145">
-        <v>-0.5100769818975097</v>
+        <v>-0.5100769818975124</v>
       </c>
       <c r="B40" t="n" s="146">
-        <v>-0.22768593916850843</v>
+        <v>-0.22768593916850932</v>
       </c>
       <c r="C40" t="n" s="147">
         <v>-0.7066503172429588</v>
       </c>
       <c r="D40" t="n" s="148">
-        <v>1.5419799271024486</v>
+        <v>1.5419799271024495</v>
       </c>
     </row>
     <row r="41">
@@ -2742,24 +2742,24 @@
         <v>0.44085823824134085</v>
       </c>
       <c r="B41" t="n" s="146">
-        <v>-0.16521922158592073</v>
+        <v>-0.16521922158591984</v>
       </c>
       <c r="C41" t="n" s="147">
-        <v>0.25227000447750036</v>
+        <v>0.2522700044774986</v>
       </c>
       <c r="D41" t="n" s="148">
-        <v>0.49326618176885795</v>
+        <v>0.49326618176885706</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n" s="145">
-        <v>0.8900058601058172</v>
+        <v>0.8900058601058163</v>
       </c>
       <c r="B42" t="n" s="146">
-        <v>0.19746084495102778</v>
+        <v>0.19746084495103045</v>
       </c>
       <c r="C42" t="n" s="147">
-        <v>-0.30113785002829196</v>
+        <v>-0.3011378500282902</v>
       </c>
       <c r="D42" t="n" s="148">
         <v>-1.0584205795024255</v>
@@ -2767,27 +2767,27 @@
     </row>
     <row r="43">
       <c r="A43" t="n" s="145">
-        <v>0.28746259796929774</v>
+        <v>0.28746259796929596</v>
       </c>
       <c r="B43" t="n" s="146">
-        <v>-0.4366423313895762</v>
+        <v>-0.4366423313895753</v>
       </c>
       <c r="C43" t="n" s="147">
-        <v>0.08612090762287217</v>
+        <v>0.08612090762287483</v>
       </c>
       <c r="D43" t="n" s="148">
-        <v>0.3407806606964181</v>
+        <v>0.3407806606964163</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n" s="145">
-        <v>0.29966016602208656</v>
+        <v>0.29966016602208523</v>
       </c>
       <c r="B44" t="n" s="146">
-        <v>-0.3932656185547918</v>
+        <v>-0.3932656185547927</v>
       </c>
       <c r="C44" t="n" s="147">
-        <v>-0.9007403760105186</v>
+        <v>-0.9007403760105182</v>
       </c>
       <c r="D44" t="n" s="148">
         <v>0.35505999989842385</v>
@@ -2798,10 +2798,10 @@
         <v>0.8900058601058163</v>
       </c>
       <c r="B45" t="n" s="146">
-        <v>0.19746084495102867</v>
+        <v>0.19746084495102956</v>
       </c>
       <c r="C45" t="n" s="147">
-        <v>0.698862149971708</v>
+        <v>0.6988621499717098</v>
       </c>
       <c r="D45" t="n" s="148">
         <v>-2.0584205795024246</v>
@@ -2809,27 +2809,27 @@
     </row>
     <row r="46">
       <c r="A46" t="n" s="145">
-        <v>1.092604654369028</v>
+        <v>1.0926046543690267</v>
       </c>
       <c r="B46" t="n" s="146">
-        <v>-0.5942987578102192</v>
+        <v>-0.5942987578102183</v>
       </c>
       <c r="C46" t="n" s="147">
-        <v>-0.10105235230757259</v>
+        <v>-0.10105235230757081</v>
       </c>
       <c r="D46" t="n" s="148">
-        <v>-0.8544294416830756</v>
+        <v>-0.854429441683076</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n" s="145">
-        <v>0.4899230181024885</v>
+        <v>0.4899230181024876</v>
       </c>
       <c r="B47" t="n" s="146">
-        <v>-0.2276859391685102</v>
+        <v>-0.22768593916850932</v>
       </c>
       <c r="C47" t="n" s="147">
-        <v>0.2933496827570403</v>
+        <v>0.2933496827570412</v>
       </c>
       <c r="D47" t="n" s="148">
         <v>-0.4580200728975514</v>
@@ -2837,55 +2837,55 @@
     </row>
     <row r="48">
       <c r="A48" t="n" s="145">
-        <v>0.09260465436902798</v>
+        <v>0.0926046543690271</v>
       </c>
       <c r="B48" t="n" s="146">
-        <v>-0.5942987578102183</v>
+        <v>-0.5942987578102175</v>
       </c>
       <c r="C48" t="n" s="147">
-        <v>-0.10105235230757259</v>
+        <v>-0.1010523523075717</v>
       </c>
       <c r="D48" t="n" s="148">
-        <v>0.14557055831692445</v>
+        <v>0.145570558316924</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n" s="145">
-        <v>-1.5100769818975097</v>
+        <v>-1.5100769818975115</v>
       </c>
       <c r="B49" t="n" s="146">
         <v>0.7723140608314907</v>
       </c>
       <c r="C49" t="n" s="147">
-        <v>-0.7066503172429588</v>
+        <v>-0.7066503172429579</v>
       </c>
       <c r="D49" t="n" s="148">
-        <v>1.5419799271024504</v>
+        <v>1.5419799271024477</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n" s="145">
-        <v>0.09260465436902798</v>
+        <v>0.0926046543690271</v>
       </c>
       <c r="B50" t="n" s="146">
-        <v>-0.5942987578102183</v>
+        <v>-0.5942987578102175</v>
       </c>
       <c r="C50" t="n" s="147">
-        <v>-0.10105235230757259</v>
+        <v>-0.1010523523075717</v>
       </c>
       <c r="D50" t="n" s="148">
-        <v>0.14557055831692445</v>
+        <v>0.145570558316924</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n" s="145">
-        <v>-1.4886689798106896</v>
+        <v>-1.488668979810691</v>
       </c>
       <c r="B51" t="n" s="146">
         <v>-0.20020000697567664</v>
       </c>
       <c r="C51" t="n" s="147">
-        <v>-0.6989827997222506</v>
+        <v>-0.6989827997222489</v>
       </c>
       <c r="D51" t="n" s="148">
         <v>1.5697447670019749</v>
@@ -2893,7 +2893,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n" s="145">
-        <v>-0.5100769818975115</v>
+        <v>-0.5100769818975124</v>
       </c>
       <c r="B52" t="n" s="146">
         <v>-0.22768593916850932</v>
@@ -2902,7 +2902,7 @@
         <v>0.2933496827570403</v>
       </c>
       <c r="D52" t="n" s="148">
-        <v>0.5419799271024486</v>
+        <v>0.5419799271024477</v>
       </c>
     </row>
     <row r="53">
@@ -2913,35 +2913,35 @@
         <v>-0.0018113377908024475</v>
       </c>
       <c r="C53" t="n" s="147">
-        <v>0.4591617785758615</v>
+        <v>0.4591617785758606</v>
       </c>
       <c r="D53" t="n" s="148">
-        <v>1.7127721682555936</v>
+        <v>1.7127721682555919</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n" s="145">
-        <v>-1.7769094939160892</v>
+        <v>-1.7769094939160874</v>
       </c>
       <c r="B54" t="n" s="146">
         <v>0.6848683713847725</v>
       </c>
       <c r="C54" t="n" s="147">
-        <v>1.0506908082225026</v>
+        <v>1.0506908082225035</v>
       </c>
       <c r="D54" t="n" s="148">
-        <v>1.271819640492775</v>
+        <v>1.2718196404927742</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n" s="145">
-        <v>-0.3099730388389048</v>
+        <v>-0.3099730388389057</v>
       </c>
       <c r="B55" t="n" s="146">
         <v>-0.01495191203126911</v>
       </c>
       <c r="C55" t="n" s="147">
-        <v>0.4974851707980559</v>
+        <v>0.49748517079805676</v>
       </c>
       <c r="D55" t="n" s="148">
         <v>-0.2586415125071646</v>
@@ -2949,100 +2949,100 @@
     </row>
     <row r="56">
       <c r="A56" t="n" s="145">
-        <v>0.08193047455106406</v>
+        <v>0.08193047455106495</v>
       </c>
       <c r="B56" t="n" s="146">
-        <v>0.3629693801357776</v>
+        <v>0.3629693801357785</v>
       </c>
       <c r="C56" t="n" s="147">
-        <v>-0.12266641253456623</v>
+        <v>-0.12266641253456445</v>
       </c>
       <c r="D56" t="n" s="148">
-        <v>0.13644044648551557</v>
+        <v>0.13644044648551468</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n" s="145">
-        <v>0.09260465436902798</v>
+        <v>0.0926046543690271</v>
       </c>
       <c r="B57" t="n" s="146">
-        <v>-0.5942987578102183</v>
+        <v>-0.5942987578102175</v>
       </c>
       <c r="C57" t="n" s="147">
-        <v>-0.10105235230757259</v>
+        <v>-0.1010523523075717</v>
       </c>
       <c r="D57" t="n" s="148">
-        <v>0.14557055831692445</v>
+        <v>0.145570558316924</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n" s="145">
-        <v>-0.5100769818975106</v>
+        <v>-0.5100769818975115</v>
       </c>
       <c r="B58" t="n" s="146">
-        <v>0.7723140608314907</v>
+        <v>0.7723140608314916</v>
       </c>
       <c r="C58" t="n" s="147">
-        <v>-0.7066503172429597</v>
+        <v>-0.7066503172429579</v>
       </c>
       <c r="D58" t="n" s="148">
-        <v>0.5419799271024486</v>
+        <v>0.5419799271024477</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n" s="145">
-        <v>0.7264216834298329</v>
+        <v>0.7264216834298325</v>
       </c>
       <c r="B59" t="n" s="146">
-        <v>-0.013456850542333143</v>
+        <v>-0.013456850542332255</v>
       </c>
       <c r="C59" t="n" s="147">
-        <v>0.5052081108418811</v>
+        <v>0.5052081108418829</v>
       </c>
       <c r="D59" t="n" s="148">
-        <v>-2.212293349030958</v>
+        <v>-2.2122933490309578</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n" s="145">
-        <v>0.007496093091980072</v>
+        <v>0.007496093091981848</v>
       </c>
       <c r="B60" t="n" s="146">
-        <v>-0.4518953897011073</v>
+        <v>-0.45189538970110643</v>
       </c>
       <c r="C60" t="n" s="147">
-        <v>0.8565217304271817</v>
+        <v>0.8565217304271826</v>
       </c>
       <c r="D60" t="n" s="148">
-        <v>1.0508730616081428</v>
+        <v>1.050873061608141</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n" s="145">
-        <v>-0.5591417617586583</v>
+        <v>-0.5591417617586574</v>
       </c>
       <c r="B61" t="n" s="146">
-        <v>0.8347807784140793</v>
+        <v>0.8347807784140802</v>
       </c>
       <c r="C61" t="n" s="147">
-        <v>1.2522700044774986</v>
+        <v>1.2522700044775004</v>
       </c>
       <c r="D61" t="n" s="148">
-        <v>-0.506733818231142</v>
+        <v>-0.5067338182311429</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n" s="145">
-        <v>0.09260465436902798</v>
+        <v>0.0926046543690271</v>
       </c>
       <c r="B62" t="n" s="146">
-        <v>-0.5942987578102183</v>
+        <v>-0.5942987578102175</v>
       </c>
       <c r="C62" t="n" s="147">
-        <v>-0.10105235230757259</v>
+        <v>-0.1010523523075717</v>
       </c>
       <c r="D62" t="n" s="148">
-        <v>0.14557055831692445</v>
+        <v>0.145570558316924</v>
       </c>
     </row>
     <row r="63">
@@ -3050,13 +3050,13 @@
         <v>1.872521991336077</v>
       </c>
       <c r="B63" t="n" s="146">
-        <v>1.1743862121869713</v>
+        <v>1.174386212186973</v>
       </c>
       <c r="C63" t="n" s="147">
-        <v>1.6682151469316642</v>
+        <v>1.6682151469316668</v>
       </c>
       <c r="D63" t="n" s="148">
-        <v>-4.072443432938685</v>
+        <v>-4.072443432938686</v>
       </c>
     </row>
     <row r="64">
@@ -3067,136 +3067,136 @@
         <v>0.423953734034785</v>
       </c>
       <c r="C64" t="n" s="147">
-        <v>0.6721087719150498</v>
+        <v>0.6721087719150489</v>
       </c>
       <c r="D64" t="n" s="148">
-        <v>0.8341936018425953</v>
+        <v>0.8341936018425944</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n" s="145">
-        <v>-0.10999413989418194</v>
+        <v>-0.10999413989418283</v>
       </c>
       <c r="B65" t="n" s="146">
-        <v>1.1974608449510287</v>
+        <v>1.1974608449510304</v>
       </c>
       <c r="C65" t="n" s="147">
-        <v>-0.3011378500282911</v>
+        <v>-0.3011378500282902</v>
       </c>
       <c r="D65" t="n" s="148">
-        <v>-1.0584205795024246</v>
+        <v>-1.0584205795024255</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n" s="145">
-        <v>0.2230905060839108</v>
+        <v>0.22309050608391345</v>
       </c>
       <c r="B66" t="n" s="146">
-        <v>-0.3151316286152275</v>
+        <v>-0.3151316286152266</v>
       </c>
       <c r="C66" t="n" s="147">
-        <v>1.0506908082225026</v>
+        <v>1.0506908082225044</v>
       </c>
       <c r="D66" t="n" s="148">
-        <v>0.27181964049277507</v>
+        <v>0.2718196404927742</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n" s="145">
-        <v>0.5113310201893104</v>
+        <v>0.5113310201893086</v>
       </c>
       <c r="B67" t="n" s="146">
-        <v>-1.2002000069756775</v>
+        <v>-1.2002000069756766</v>
       </c>
       <c r="C67" t="n" s="147">
         <v>-0.6989827997222497</v>
       </c>
       <c r="D67" t="n" s="148">
-        <v>0.5697447670019753</v>
+        <v>0.5697447670019749</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n" s="145">
-        <v>-0.10999413989418283</v>
+        <v>-0.10999413989418372</v>
       </c>
       <c r="B68" t="n" s="146">
-        <v>0.19746084495102778</v>
+        <v>0.19746084495103045</v>
       </c>
       <c r="C68" t="n" s="147">
-        <v>-0.30113785002829285</v>
+        <v>-0.3011378500282902</v>
       </c>
       <c r="D68" t="n" s="148">
-        <v>-0.05842057950242552</v>
+        <v>-0.058420579502426406</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n" s="145">
-        <v>1.2230905060839108</v>
+        <v>1.2230905060839117</v>
       </c>
       <c r="B69" t="n" s="146">
-        <v>0.6848683713847734</v>
+        <v>0.6848683713847725</v>
       </c>
       <c r="C69" t="n" s="147">
         <v>-0.9493091917774965</v>
       </c>
       <c r="D69" t="n" s="148">
-        <v>0.2718196404927742</v>
+        <v>0.2718196404927733</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n" s="145">
-        <v>-0.5591417617586592</v>
+        <v>-0.5591417617586574</v>
       </c>
       <c r="B70" t="n" s="146">
-        <v>-0.16521922158591895</v>
+        <v>-0.16521922158591984</v>
       </c>
       <c r="C70" t="n" s="147">
         <v>0.25227000447750036</v>
       </c>
       <c r="D70" t="n" s="148">
-        <v>1.493266181768858</v>
+        <v>1.4932661817688562</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n" s="145">
-        <v>1.2230905060839108</v>
+        <v>1.2230905060839135</v>
       </c>
       <c r="B71" t="n" s="146">
-        <v>-0.3151316286152266</v>
+        <v>-0.3151316286152275</v>
       </c>
       <c r="C71" t="n" s="147">
-        <v>-0.9493091917774965</v>
+        <v>-0.9493091917774956</v>
       </c>
       <c r="D71" t="n" s="148">
-        <v>1.2718196404927733</v>
+        <v>1.2718196404927742</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n" s="145">
-        <v>0.9444274581661412</v>
+        <v>0.9444274581661403</v>
       </c>
       <c r="B72" t="n" s="146">
-        <v>0.1711034420855957</v>
+        <v>0.17110344208559658</v>
       </c>
       <c r="C72" t="n" s="147">
-        <v>-0.28635032084936496</v>
+        <v>-0.28635032084936407</v>
       </c>
       <c r="D72" t="n" s="148">
-        <v>-1.992244555752262</v>
+        <v>-1.9922445557522614</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n" s="145">
-        <v>-0.5100769818975106</v>
+        <v>-0.5100769818975115</v>
       </c>
       <c r="B73" t="n" s="146">
-        <v>1.7723140608314907</v>
+        <v>1.7723140608314898</v>
       </c>
       <c r="C73" t="n" s="147">
-        <v>-0.7066503172429597</v>
+        <v>-0.7066503172429588</v>
       </c>
       <c r="D73" t="n" s="148">
-        <v>-0.45802007289755053</v>
+        <v>-0.4580200728975523</v>
       </c>
     </row>
     <row r="74">
@@ -3207,7 +3207,7 @@
         <v>2.1974608449510296</v>
       </c>
       <c r="C74" t="n" s="147">
-        <v>0.698862149971708</v>
+        <v>0.6988621499717089</v>
       </c>
       <c r="D74" t="n" s="148">
         <v>-3.0584205795024255</v>
@@ -3215,13 +3215,13 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="145">
-        <v>-0.48866897981068913</v>
+        <v>-0.48866897981069</v>
       </c>
       <c r="B75" t="n" s="146">
-        <v>0.7997999930243216</v>
+        <v>0.7997999930243234</v>
       </c>
       <c r="C75" t="n" s="147">
-        <v>0.30101720027775114</v>
+        <v>0.3010172002777516</v>
       </c>
       <c r="D75" t="n" s="148">
         <v>-1.4302552329980243</v>
@@ -3229,27 +3229,27 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="145">
-        <v>0.9444274581661412</v>
+        <v>0.9444274581661407</v>
       </c>
       <c r="B76" t="n" s="146">
-        <v>-0.8288965579144034</v>
+        <v>-0.8288965579144039</v>
       </c>
       <c r="C76" t="n" s="147">
         <v>-0.28635032084936496</v>
       </c>
       <c r="D76" t="n" s="148">
-        <v>-0.9922445557522623</v>
+        <v>-0.9922445557522614</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n" s="145">
-        <v>0.29966016602208656</v>
+        <v>0.29966016602208523</v>
       </c>
       <c r="B77" t="n" s="146">
-        <v>-0.3932656185547927</v>
+        <v>-0.3932656185547918</v>
       </c>
       <c r="C77" t="n" s="147">
-        <v>0.09925962398948096</v>
+        <v>0.09925962398948274</v>
       </c>
       <c r="D77" t="n" s="148">
         <v>-0.6449400001015761</v>
@@ -3263,24 +3263,24 @@
         <v>1.1743862121869713</v>
       </c>
       <c r="C78" t="n" s="147">
-        <v>-1.331784853068335</v>
+        <v>-1.331784853068334</v>
       </c>
       <c r="D78" t="n" s="148">
-        <v>1.9275565670613144</v>
+        <v>1.9275565670613135</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n" s="145">
-        <v>-0.10999413989418283</v>
+        <v>-0.10999413989418372</v>
       </c>
       <c r="B79" t="n" s="146">
-        <v>0.19746084495102778</v>
+        <v>0.19746084495103045</v>
       </c>
       <c r="C79" t="n" s="147">
-        <v>-0.30113785002829285</v>
+        <v>-0.3011378500282902</v>
       </c>
       <c r="D79" t="n" s="148">
-        <v>-0.05842057950242552</v>
+        <v>-0.058420579502426406</v>
       </c>
     </row>
     <row r="80">
@@ -3288,24 +3288,24 @@
         <v>0.44085823824134085</v>
       </c>
       <c r="B80" t="n" s="146">
-        <v>-0.16521922158592073</v>
+        <v>-0.16521922158591984</v>
       </c>
       <c r="C80" t="n" s="147">
-        <v>0.25227000447750036</v>
+        <v>0.2522700044774986</v>
       </c>
       <c r="D80" t="n" s="148">
-        <v>0.49326618176885795</v>
+        <v>0.49326618176885706</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n" s="145">
-        <v>0.0074960930919791835</v>
+        <v>0.00749609309198096</v>
       </c>
       <c r="B81" t="n" s="146">
-        <v>0.5481046102988936</v>
+        <v>0.5481046102988918</v>
       </c>
       <c r="C81" t="n" s="147">
-        <v>0.8565217304271826</v>
+        <v>0.8565217304271835</v>
       </c>
       <c r="D81" t="n" s="148">
         <v>0.050873061608142756</v>
@@ -3313,41 +3313,41 @@
     </row>
     <row r="82">
       <c r="A82" t="n" s="145">
-        <v>-1.7003398339779134</v>
+        <v>-1.7003398339779143</v>
       </c>
       <c r="B82" t="n" s="146">
-        <v>-0.3932656185547927</v>
+        <v>-0.3932656185547918</v>
       </c>
       <c r="C82" t="n" s="147">
-        <v>0.0992596239894814</v>
+        <v>0.09925962398948274</v>
       </c>
       <c r="D82" t="n" s="148">
-        <v>1.3550599998984243</v>
+        <v>1.3550599998984239</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n" s="145">
-        <v>-1.2056170010856966</v>
+        <v>-1.205617001085697</v>
       </c>
       <c r="B83" t="n" s="146">
-        <v>-1.0315404524880227</v>
+        <v>-1.0315404524880218</v>
       </c>
       <c r="C83" t="n" s="147">
-        <v>0.5728565092008684</v>
+        <v>0.5728565092008693</v>
       </c>
       <c r="D83" t="n" s="148">
-        <v>-0.14904787547706055</v>
+        <v>-0.1490478754770601</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n" s="145">
-        <v>0.09260465436902754</v>
+        <v>0.0926046543690271</v>
       </c>
       <c r="B84" t="n" s="146">
-        <v>-0.5942987578102192</v>
+        <v>-0.5942987578102183</v>
       </c>
       <c r="C84" t="n" s="147">
-        <v>0.8989476476924283</v>
+        <v>0.8989476476924292</v>
       </c>
       <c r="D84" t="n" s="148">
         <v>-0.854429441683076</v>
@@ -3355,16 +3355,16 @@
     </row>
     <row r="85">
       <c r="A85" t="n" s="145">
-        <v>-1.407750080746097</v>
+        <v>-1.4077500807460974</v>
       </c>
       <c r="B85" t="n" s="146">
         <v>0.7531241885584983</v>
       </c>
       <c r="C85" t="n" s="147">
-        <v>-1.641408785464384</v>
+        <v>-1.641408785464383</v>
       </c>
       <c r="D85" t="n" s="148">
-        <v>0.6530952077204693</v>
+        <v>0.6530952077204697</v>
       </c>
     </row>
     <row r="86">
@@ -3372,38 +3372,38 @@
         <v>0.8725219913360762</v>
       </c>
       <c r="B86" t="n" s="146">
-        <v>-1.825613787813027</v>
+        <v>-1.8256137878130279</v>
       </c>
       <c r="C86" t="n" s="147">
         <v>-0.33178485306833405</v>
       </c>
       <c r="D86" t="n" s="148">
-        <v>1.9275565670613153</v>
+        <v>1.9275565670613126</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n" s="145">
-        <v>-0.8355649812936217</v>
+        <v>-0.835564981293623</v>
       </c>
       <c r="B87" t="n" s="146">
-        <v>0.358372790677703</v>
+        <v>0.35837279067770345</v>
       </c>
       <c r="C87" t="n" s="147">
-        <v>-1.0726870386490934</v>
+        <v>-1.0726870386490925</v>
       </c>
       <c r="D87" t="n" s="148">
-        <v>0.22853382801366617</v>
+        <v>0.22853382801366573</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n" s="145">
-        <v>-0.40775008074609653</v>
+        <v>-0.4077500807460974</v>
       </c>
       <c r="B88" t="n" s="146">
-        <v>-0.24687581144150217</v>
+        <v>-0.24687581144150306</v>
       </c>
       <c r="C88" t="n" s="147">
-        <v>-0.641408785464384</v>
+        <v>-0.6414087854643831</v>
       </c>
       <c r="D88" t="n" s="148">
         <v>-0.3469047922795303</v>
@@ -3414,41 +3414,41 @@
         <v>1.6900269611610943</v>
       </c>
       <c r="B89" t="n" s="146">
-        <v>-0.014951912031269998</v>
+        <v>-0.014951912031268222</v>
       </c>
       <c r="C89" t="n" s="147">
-        <v>-0.502514829201945</v>
+        <v>-0.5025148292019423</v>
       </c>
       <c r="D89" t="n" s="148">
-        <v>-1.2586415125071646</v>
+        <v>-1.2586415125071637</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n" s="145">
-        <v>0.299660166022087</v>
+        <v>0.29966016602208434</v>
       </c>
       <c r="B90" t="n" s="146">
         <v>-1.3932656185547927</v>
       </c>
       <c r="C90" t="n" s="147">
-        <v>0.09925962398948185</v>
+        <v>0.0992596239894814</v>
       </c>
       <c r="D90" t="n" s="148">
-        <v>0.3550599998984252</v>
+        <v>0.3550599998984234</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n" s="145">
-        <v>0.299660166022087</v>
+        <v>0.29966016602208434</v>
       </c>
       <c r="B91" t="n" s="146">
         <v>-1.3932656185547927</v>
       </c>
       <c r="C91" t="n" s="147">
-        <v>0.09925962398948185</v>
+        <v>0.0992596239894814</v>
       </c>
       <c r="D91" t="n" s="148">
-        <v>0.3550599998984252</v>
+        <v>0.3550599998984234</v>
       </c>
     </row>
     <row r="92">
@@ -3758,28 +3758,28 @@
         <v>4.392857142857143</v>
       </c>
       <c r="D6" t="n" s="194">
-        <v>-1.4101149227797947</v>
+        <v>-1.4101149227798147</v>
       </c>
       <c r="E6" t="n" s="195">
-        <v>-7.952960283773328</v>
+        <v>-7.952960283773473</v>
       </c>
       <c r="F6" t="n" s="196">
-        <v>-9.838253403963593</v>
+        <v>-9.838253403963735</v>
       </c>
       <c r="G6" t="n" s="197">
-        <v>-11.302540240245367</v>
+        <v>-11.302540240245508</v>
       </c>
       <c r="H6" t="n" s="198">
-        <v>-13.020559873072763</v>
+        <v>-13.020559873072905</v>
       </c>
       <c r="I6" t="n" s="199">
-        <v>-12.27009438037743</v>
+        <v>-12.270094380377571</v>
       </c>
       <c r="J6" t="n" s="200">
-        <v>-11.518278288462</v>
+        <v>-11.518278288462142</v>
       </c>
       <c r="K6" t="n" s="201">
-        <v>-9.870804459458563</v>
+        <v>-9.870804459458702</v>
       </c>
       <c r="L6" t="n" s="202">
         <v>1.0</v>
@@ -3814,28 +3814,28 @@
         <v>5.071428571428571</v>
       </c>
       <c r="D7" t="n" s="194">
-        <v>-2.1026461243129475</v>
+        <v>-2.102646124312966</v>
       </c>
       <c r="E7" t="n" s="195">
-        <v>-8.645491485306481</v>
+        <v>-8.645491485306625</v>
       </c>
       <c r="F7" t="n" s="196">
-        <v>-11.223315807029898</v>
+        <v>-11.223315807030037</v>
       </c>
       <c r="G7" t="n" s="197">
-        <v>-13.380133844844826</v>
+        <v>-13.380133844844963</v>
       </c>
       <c r="H7" t="n" s="198">
-        <v>-15.790684679205375</v>
+        <v>-15.790684679205512</v>
       </c>
       <c r="I7" t="n" s="199">
-        <v>-15.732750388043197</v>
+        <v>-15.732750388043332</v>
       </c>
       <c r="J7" t="n" s="200">
-        <v>-15.67346549766092</v>
+        <v>-15.673465497661052</v>
       </c>
       <c r="K7" t="n" s="201">
-        <v>-14.718522870190633</v>
+        <v>-14.718522870190764</v>
       </c>
       <c r="L7" t="n" s="202">
         <v>1.0</v>
@@ -3870,28 +3870,28 @@
         <v>4.589285714285714</v>
       </c>
       <c r="D8" t="n" s="194">
-        <v>-1.6044053855522058</v>
+        <v>-1.604405385552225</v>
       </c>
       <c r="E8" t="n" s="195">
-        <v>-8.147250746545739</v>
+        <v>-8.147250746545884</v>
       </c>
       <c r="F8" t="n" s="196">
-        <v>-10.226834329508415</v>
+        <v>-10.226834329508556</v>
       </c>
       <c r="G8" t="n" s="197">
-        <v>-11.8854116285626</v>
+        <v>-11.88541162856274</v>
       </c>
       <c r="H8" t="n" s="198">
-        <v>-13.797721724162407</v>
+        <v>-13.797721724162546</v>
       </c>
       <c r="I8" t="n" s="199">
-        <v>-13.241546694239485</v>
+        <v>-13.241546694239624</v>
       </c>
       <c r="J8" t="n" s="200">
-        <v>-12.684021065096474</v>
+        <v>-12.684021065096605</v>
       </c>
       <c r="K8" t="n" s="201">
-        <v>-11.230837698865441</v>
+        <v>-11.230837698865574</v>
       </c>
       <c r="L8" t="n" s="202">
         <v>1.0</v>
@@ -3926,28 +3926,28 @@
         <v>4.339285714285714</v>
       </c>
       <c r="D9" t="n" s="194">
-        <v>-1.357925974145625</v>
+        <v>-1.3579259741456453</v>
       </c>
       <c r="E9" t="n" s="195">
-        <v>-7.900771335139159</v>
+        <v>-7.900771335139304</v>
       </c>
       <c r="F9" t="n" s="196">
-        <v>-9.733875506695254</v>
+        <v>-9.733875506695396</v>
       </c>
       <c r="G9" t="n" s="197">
-        <v>-11.14597339434286</v>
+        <v>-11.145973394343</v>
       </c>
       <c r="H9" t="n" s="198">
-        <v>-12.811804078536086</v>
+        <v>-12.811804078536227</v>
       </c>
       <c r="I9" t="n" s="199">
-        <v>-12.009149637206583</v>
+        <v>-12.009149637206725</v>
       </c>
       <c r="J9" t="n" s="200">
-        <v>-11.205144596656986</v>
+        <v>-11.205144596657124</v>
       </c>
       <c r="K9" t="n" s="201">
-        <v>-9.505481819019376</v>
+        <v>-9.505481819019517</v>
       </c>
       <c r="L9" t="n" s="202">
         <v>1.0</v>
@@ -4140,7 +4140,7 @@
         <v>31</v>
       </c>
       <c r="B22" t="n" s="252">
-        <v>-0.9051252803137024</v>
+        <v>-0.9051252803137023</v>
       </c>
     </row>
     <row r="23">
@@ -4148,7 +4148,7 @@
         <v>32</v>
       </c>
       <c r="B23" t="n" s="252">
-        <v>-1.6009399303108673</v>
+        <v>-1.6009399303108658</v>
       </c>
     </row>
     <row r="24">
@@ -4156,7 +4156,7 @@
         <v>33</v>
       </c>
       <c r="B24" t="n" s="252">
-        <v>-1.1111949942532806</v>
+        <v>-1.111194994253279</v>
       </c>
     </row>
     <row r="25">
@@ -4164,7 +4164,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="n" s="252">
-        <v>-0.8531085204707997</v>
+        <v>-0.8531085204707987</v>
       </c>
     </row>
     <row r="26">
@@ -4216,28 +4216,28 @@
         <v>31</v>
       </c>
       <c r="B30" t="n" s="272">
-        <v>0.8963600570914151</v>
+        <v>0.9185923197528153</v>
       </c>
       <c r="C30" t="n" s="273">
-        <v>-0.5215389714943105</v>
+        <v>-0.41026154800055953</v>
       </c>
       <c r="D30" t="n" s="274">
-        <v>0.6019913645146439</v>
+        <v>0.6816140958126913</v>
       </c>
       <c r="E30" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F30" t="n" s="276">
-        <v>0.8873367446801429</v>
+        <v>0.9111463392901317</v>
       </c>
       <c r="G30" t="n" s="277">
-        <v>-0.5815614464164797</v>
+        <v>-0.4585214211406812</v>
       </c>
       <c r="H30" t="n" s="278">
-        <v>0.5608621180592315</v>
+        <v>0.6465778763078986</v>
       </c>
       <c r="I30" t="n" s="279">
-        <v>0.5608621180592315</v>
+        <v>0.6465778763078986</v>
       </c>
     </row>
     <row r="31">
@@ -4245,28 +4245,28 @@
         <v>32</v>
       </c>
       <c r="B31" t="n" s="272">
-        <v>0.7824656287301153</v>
+        <v>0.7936137408035653</v>
       </c>
       <c r="C31" t="n" s="273">
-        <v>-1.1411764928448849</v>
+        <v>-1.0834171744895056</v>
       </c>
       <c r="D31" t="n" s="274">
-        <v>0.25379648453446324</v>
+        <v>0.2786232959063671</v>
       </c>
       <c r="E31" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F31" t="n" s="276">
-        <v>0.7861598256250322</v>
+        <v>0.7893952382734333</v>
       </c>
       <c r="G31" t="n" s="277">
-        <v>-1.1716343056946417</v>
+        <v>-1.1561833615139476</v>
       </c>
       <c r="H31" t="n" s="278">
-        <v>0.24134390865217722</v>
+        <v>0.24760616401839625</v>
       </c>
       <c r="I31" t="n" s="279">
-        <v>0.48268781730435445</v>
+        <v>0.4952123280367925</v>
       </c>
     </row>
     <row r="32">
@@ -4274,28 +4274,28 @@
         <v>33</v>
       </c>
       <c r="B32" t="n" s="272">
-        <v>0.6623665298551001</v>
+        <v>0.6626271997229916</v>
       </c>
       <c r="C32" t="n" s="273">
-        <v>-1.9360825665778498</v>
+        <v>-1.9360221966989721</v>
       </c>
       <c r="D32" t="n" s="274">
-        <v>0.05285758934339827</v>
+        <v>0.05286498246106212</v>
       </c>
       <c r="E32" t="n" s="275">
-        <v>0.47571830409058447</v>
+        <v>0.4757848421495591</v>
       </c>
       <c r="F32" t="n" s="276">
-        <v>0.6481748681926544</v>
+        <v>0.6535124953082828</v>
       </c>
       <c r="G32" t="n" s="277">
-        <v>-2.0940655388135236</v>
+        <v>-2.0590228257324448</v>
       </c>
       <c r="H32" t="n" s="278">
-        <v>0.03625414238853233</v>
+        <v>0.03949205191939344</v>
       </c>
       <c r="I32" t="n" s="279">
-        <v>0.10876242716559698</v>
+        <v>0.11847615575818031</v>
       </c>
     </row>
     <row r="33">
@@ -4303,28 +4303,28 @@
         <v>34</v>
       </c>
       <c r="B33" t="n" s="272">
-        <v>1.5983266790393118</v>
+        <v>1.5938693042674448</v>
       </c>
       <c r="C33" t="n" s="273">
-        <v>2.6681483360239375</v>
+        <v>2.6440918508615527</v>
       </c>
       <c r="D33" t="n" s="274">
-        <v>0.007627057608106231</v>
+        <v>0.008191042554212857</v>
       </c>
       <c r="E33" t="n" s="275">
-        <v>0.0762705760810623</v>
+        <v>0.08191042554212857</v>
       </c>
       <c r="F33" t="n" s="276">
-        <v>1.6119663791671812</v>
+        <v>1.5979035627528566</v>
       </c>
       <c r="G33" t="n" s="277">
-        <v>2.8022141869022215</v>
+        <v>2.7397563831386544</v>
       </c>
       <c r="H33" t="n" s="278">
-        <v>0.005075316544865756</v>
+        <v>0.006148473954920521</v>
       </c>
       <c r="I33" t="n" s="279">
-        <v>0.020301266179463023</v>
+        <v>0.024593895819682084</v>
       </c>
     </row>
     <row r="34">
@@ -4332,28 +4332,28 @@
         <v>57</v>
       </c>
       <c r="B34" t="n" s="272">
-        <v>1.381429584828628</v>
+        <v>1.2475183121645228</v>
       </c>
       <c r="C34" t="n" s="273">
-        <v>1.599640051457245</v>
+        <v>1.5738387485738259</v>
       </c>
       <c r="D34" t="n" s="274">
-        <v>0.10967845798138334</v>
+        <v>0.11552473336663306</v>
       </c>
       <c r="E34" t="n" s="275">
-        <v>0.8774276638510667</v>
+        <v>0.9241978669330645</v>
       </c>
       <c r="F34" t="n" s="276">
-        <v>1.5128341295586478</v>
+        <v>1.4652716174951272</v>
       </c>
       <c r="G34" t="n" s="277">
-        <v>3.2712113632684425</v>
+        <v>2.935485073413053</v>
       </c>
       <c r="H34" t="n" s="278">
-        <v>0.001070878412578528</v>
+        <v>0.0033302663339079093</v>
       </c>
       <c r="I34" t="n" s="279">
-        <v>0.005354392062892639</v>
+        <v>0.016651331669539547</v>
       </c>
     </row>
     <row r="35">
@@ -4361,28 +4361,28 @@
         <v>58</v>
       </c>
       <c r="B35" t="n" s="272">
-        <v>1.9643075658963116</v>
+        <v>1.8544861899868517</v>
       </c>
       <c r="C35" t="n" s="273">
-        <v>1.0282653860292317</v>
+        <v>0.961121488356128</v>
       </c>
       <c r="D35" t="n" s="274">
-        <v>0.30382500856285344</v>
+        <v>0.3364910863881247</v>
       </c>
       <c r="E35" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F35" t="n" s="276">
-        <v>1.7709909003367088</v>
+        <v>1.7006240957540704</v>
       </c>
       <c r="G35" t="n" s="277">
-        <v>5.026672354109598</v>
+        <v>4.625404710765651</v>
       </c>
       <c r="H35" t="n" s="278">
-        <v>4.990639491289459E-7</v>
+        <v>3.7386766054784034E-6</v>
       </c>
       <c r="I35" t="n" s="279">
-        <v>3.9925115930315676E-6</v>
+        <v>2.9909412843827227E-5</v>
       </c>
     </row>
     <row r="36">
@@ -4390,28 +4390,28 @@
         <v>59</v>
       </c>
       <c r="B36" t="n" s="272">
-        <v>1.6347684170888916</v>
+        <v>1.5771703856817247</v>
       </c>
       <c r="C36" t="n" s="273">
-        <v>0.9644285911109184</v>
+        <v>0.9020803970337582</v>
       </c>
       <c r="D36" t="n" s="274">
-        <v>0.3348310936447223</v>
+        <v>0.3670141613828799</v>
       </c>
       <c r="E36" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F36" t="n" s="276">
-        <v>1.5126120297620933</v>
+        <v>1.4855193256016759</v>
       </c>
       <c r="G36" t="n" s="277">
-        <v>4.1713674835082095</v>
+        <v>3.9438786883434767</v>
       </c>
       <c r="H36" t="n" s="278">
-        <v>3.027771173255964E-5</v>
+        <v>8.017422643765382E-5</v>
       </c>
       <c r="I36" t="n" s="279">
-        <v>2.1194398212791749E-4</v>
+        <v>5.612195850635767E-4</v>
       </c>
     </row>
     <row r="37">
@@ -4419,28 +4419,28 @@
         <v>60</v>
       </c>
       <c r="B37" t="n" s="272">
-        <v>1.335928183093764</v>
+        <v>1.3308692640018553</v>
       </c>
       <c r="C37" t="n" s="273">
-        <v>0.8443330064121967</v>
+        <v>0.8293289714948423</v>
       </c>
       <c r="D37" t="n" s="274">
-        <v>0.3984833469723245</v>
+        <v>0.40691828141060116</v>
       </c>
       <c r="E37" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F37" t="n" s="276">
-        <v>1.30542237467969</v>
+        <v>1.297754692199495</v>
       </c>
       <c r="G37" t="n" s="277">
-        <v>3.446351345345648</v>
+        <v>3.34977472867429</v>
       </c>
       <c r="H37" t="n" s="278">
-        <v>5.682110841100512E-4</v>
+        <v>8.0877307221796E-4</v>
       </c>
       <c r="I37" t="n" s="279">
-        <v>0.003409266504660307</v>
+        <v>0.00485263843330776</v>
       </c>
     </row>
     <row r="38">
@@ -4448,28 +4448,28 @@
         <v>61</v>
       </c>
       <c r="B38" t="n" s="272">
-        <v>1.395822963875088</v>
+        <v>1.4286261021125053</v>
       </c>
       <c r="C38" t="n" s="273">
-        <v>0.7445061807855308</v>
+        <v>0.8014382422986912</v>
       </c>
       <c r="D38" t="n" s="274">
-        <v>0.45657030336065746</v>
+        <v>0.4228779833715728</v>
       </c>
       <c r="E38" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F38" t="n" s="276">
-        <v>1.5104821466217802</v>
+        <v>1.534082342445606</v>
       </c>
       <c r="G38" t="n" s="277">
-        <v>8.222992799769756</v>
+        <v>8.585609445542032</v>
       </c>
       <c r="H38" t="n" s="278">
-        <v>1.9848675510000352E-16</v>
+        <v>9.035613750983924E-18</v>
       </c>
       <c r="I38" t="n" s="279">
-        <v>1.9848675510000353E-15</v>
+        <v>9.035613750983925E-17</v>
       </c>
     </row>
     <row r="39">
@@ -4477,28 +4477,28 @@
         <v>62</v>
       </c>
       <c r="B39" t="n" s="272">
-        <v>1.2052173971569304</v>
+        <v>1.237463681936439</v>
       </c>
       <c r="C39" t="n" s="273">
-        <v>1.283140764604642</v>
+        <v>1.2467942402534915</v>
       </c>
       <c r="D39" t="n" s="274">
-        <v>0.19944276430340152</v>
+        <v>0.2124729529624044</v>
       </c>
       <c r="E39" t="n" s="275">
         <v>1.0</v>
       </c>
       <c r="F39" t="n" s="276">
-        <v>1.6917258000307853</v>
+        <v>1.7152499654561557</v>
       </c>
       <c r="G39" t="n" s="277">
-        <v>5.935022843317836</v>
+        <v>6.119447882150322</v>
       </c>
       <c r="H39" t="n" s="278">
-        <v>2.9380458972905485E-9</v>
+        <v>9.390013514069407E-10</v>
       </c>
       <c r="I39" t="n" s="279">
-        <v>2.6442413075614938E-8</v>
+        <v>8.451012162662466E-9</v>
       </c>
     </row>
     <row r="40">
@@ -5915,16 +5915,16 @@
         <v>1.0</v>
       </c>
       <c r="G2" t="n" s="304">
-        <v>0.5541001462555222</v>
+        <v>0.5541001462555216</v>
       </c>
       <c r="H2" t="n" s="305">
-        <v>-0.7463463445150715</v>
+        <v>-0.7463463445150745</v>
       </c>
       <c r="I2" t="n" s="306">
-        <v>0.586657061125332</v>
+        <v>0.5866570611253308</v>
       </c>
       <c r="J2" t="n" s="307">
-        <v>-0.6744600626245147</v>
+        <v>-0.6744600626245181</v>
       </c>
     </row>
     <row r="3">
@@ -5947,16 +5947,16 @@
         <v>2.0</v>
       </c>
       <c r="G3" t="n" s="304">
-        <v>0.15004320122945594</v>
+        <v>0.1500432012294557</v>
       </c>
       <c r="H3" t="n" s="305">
-        <v>-1.8067106976315266</v>
+        <v>-1.8067106976315317</v>
       </c>
       <c r="I3" t="n" s="306">
-        <v>0.1459326462159756</v>
+        <v>0.14593264621597538</v>
       </c>
       <c r="J3" t="n" s="307">
-        <v>-1.8593634750082222</v>
+        <v>-1.8593634750082266</v>
       </c>
     </row>
     <row r="4">
@@ -5979,16 +5979,16 @@
         <v>3.0</v>
       </c>
       <c r="G4" t="n" s="304">
-        <v>0.07974967425702942</v>
+        <v>0.07974967425702918</v>
       </c>
       <c r="H4" t="n" s="305">
-        <v>-2.37847550319841</v>
+        <v>-2.3784755031984264</v>
       </c>
       <c r="I4" t="n" s="306">
-        <v>0.07227735714710204</v>
+        <v>0.07227735714710273</v>
       </c>
       <c r="J4" t="n" s="307">
-        <v>-2.553058239296056</v>
+        <v>-2.5530582392960635</v>
       </c>
     </row>
     <row r="5">
@@ -6011,16 +6011,16 @@
         <v>4.0</v>
       </c>
       <c r="G5" t="n" s="304">
-        <v>0.45048683348909685</v>
+        <v>0.45048683348909646</v>
       </c>
       <c r="H5" t="n" s="305">
-        <v>-1.0155012136807222</v>
+        <v>-1.0155012136807235</v>
       </c>
       <c r="I5" t="n" s="306">
-        <v>0.457838913470001</v>
+        <v>0.45783891347000044</v>
       </c>
       <c r="J5" t="n" s="307">
-        <v>-0.9942876716116342</v>
+        <v>-0.994287671611636</v>
       </c>
     </row>
     <row r="6">
@@ -6043,16 +6043,16 @@
         <v>5.0</v>
       </c>
       <c r="G6" t="n" s="304">
-        <v>0.8084461347065071</v>
+        <v>0.8084461347065058</v>
       </c>
       <c r="H6" t="n" s="305">
-        <v>-0.06732912467597535</v>
+        <v>-0.06732912467597815</v>
       </c>
       <c r="I6" t="n" s="306">
-        <v>0.774121821553641</v>
+        <v>0.7741218215536403</v>
       </c>
       <c r="J6" t="n" s="307">
-        <v>-0.1334579753047425</v>
+        <v>-0.1334579753047442</v>
       </c>
     </row>
     <row r="7">
@@ -6075,16 +6075,16 @@
         <v>6.0</v>
       </c>
       <c r="G7" t="n" s="304">
-        <v>0.07974967425702942</v>
+        <v>0.07974967425702918</v>
       </c>
       <c r="H7" t="n" s="305">
-        <v>-2.37847550319841</v>
+        <v>-2.3784755031984264</v>
       </c>
       <c r="I7" t="n" s="306">
-        <v>0.07227735714710204</v>
+        <v>0.07227735714710273</v>
       </c>
       <c r="J7" t="n" s="307">
-        <v>-2.553058239296056</v>
+        <v>-2.5530582392960635</v>
       </c>
     </row>
     <row r="8">
@@ -6107,16 +6107,16 @@
         <v>7.0</v>
       </c>
       <c r="G8" t="n" s="304">
-        <v>0.5560357319983331</v>
+        <v>0.5560357319983334</v>
       </c>
       <c r="H8" t="n" s="305">
-        <v>-0.3523817927033834</v>
+        <v>-0.35238179270338144</v>
       </c>
       <c r="I8" t="n" s="306">
-        <v>0.5400266491166908</v>
+        <v>0.5400266491166917</v>
       </c>
       <c r="J8" t="n" s="307">
-        <v>-0.3904224794435678</v>
+        <v>-0.39042247944356434</v>
       </c>
     </row>
     <row r="9">
@@ -6139,16 +6139,16 @@
         <v>8.0</v>
       </c>
       <c r="G9" t="n" s="304">
-        <v>0.09874673103096943</v>
+        <v>0.0987467310309691</v>
       </c>
       <c r="H9" t="n" s="305">
-        <v>-2.3928717806761903</v>
+        <v>-2.3928717806761886</v>
       </c>
       <c r="I9" t="n" s="306">
-        <v>0.0989458798360156</v>
+        <v>0.09894587983601541</v>
       </c>
       <c r="J9" t="n" s="307">
-        <v>-2.40005846022936</v>
+        <v>-2.4000584602293564</v>
       </c>
     </row>
     <row r="10">
@@ -6171,16 +6171,16 @@
         <v>9.0</v>
       </c>
       <c r="G10" t="n" s="304">
-        <v>0.25639259233803396</v>
+        <v>0.25639259233803385</v>
       </c>
       <c r="H10" t="n" s="305">
-        <v>-1.1034440952272264</v>
+        <v>-1.1034440952272249</v>
       </c>
       <c r="I10" t="n" s="306">
-        <v>0.2616488946119843</v>
+        <v>0.26164889461198404</v>
       </c>
       <c r="J10" t="n" s="307">
-        <v>-1.103890000584773</v>
+        <v>-1.1038900005847718</v>
       </c>
     </row>
     <row r="11">
@@ -6203,16 +6203,16 @@
         <v>10.0</v>
       </c>
       <c r="G11" t="n" s="304">
-        <v>1.5246336201961157</v>
+        <v>1.5246336201961177</v>
       </c>
       <c r="H11" t="n" s="305">
-        <v>0.8184640837087596</v>
+        <v>0.8184640837087608</v>
       </c>
       <c r="I11" t="n" s="306">
-        <v>1.478608103915084</v>
+        <v>1.4786081039150878</v>
       </c>
       <c r="J11" t="n" s="307">
-        <v>0.7790224679805356</v>
+        <v>0.7790224679805384</v>
       </c>
     </row>
     <row r="12">
@@ -6235,16 +6235,16 @@
         <v>11.0</v>
       </c>
       <c r="G12" t="n" s="304">
-        <v>0.5599164596107509</v>
+        <v>0.5599164596107508</v>
       </c>
       <c r="H12" t="n" s="305">
-        <v>-0.3364509952669889</v>
+        <v>-0.33645099526698796</v>
       </c>
       <c r="I12" t="n" s="306">
         <v>0.570228941699287</v>
       </c>
       <c r="J12" t="n" s="307">
-        <v>-0.3191418659931947</v>
+        <v>-0.3191418659931938</v>
       </c>
     </row>
     <row r="13">
@@ -6267,16 +6267,16 @@
         <v>12.0</v>
       </c>
       <c r="G13" t="n" s="304">
-        <v>0.15004320122945594</v>
+        <v>0.1500432012294557</v>
       </c>
       <c r="H13" t="n" s="305">
-        <v>-1.8067106976315266</v>
+        <v>-1.8067106976315317</v>
       </c>
       <c r="I13" t="n" s="306">
-        <v>0.1459326462159756</v>
+        <v>0.14593264621597538</v>
       </c>
       <c r="J13" t="n" s="307">
-        <v>-1.8593634750082222</v>
+        <v>-1.8593634750082266</v>
       </c>
     </row>
     <row r="14">
@@ -6299,16 +6299,16 @@
         <v>13.0</v>
       </c>
       <c r="G14" t="n" s="304">
-        <v>0.07795368425375317</v>
+        <v>0.0779536842537526</v>
       </c>
       <c r="H14" t="n" s="305">
-        <v>-1.736774331582869</v>
+        <v>-1.73677433158287</v>
       </c>
       <c r="I14" t="n" s="306">
-        <v>0.07823064004534765</v>
+        <v>0.07823064004534709</v>
       </c>
       <c r="J14" t="n" s="307">
-        <v>-1.7361076610566921</v>
+        <v>-1.7361076610566932</v>
       </c>
     </row>
     <row r="15">
@@ -6334,13 +6334,13 @@
         <v>1.4289303832400944</v>
       </c>
       <c r="H15" t="n" s="305">
-        <v>0.7792060404942487</v>
+        <v>0.7792060404942492</v>
       </c>
       <c r="I15" t="n" s="306">
-        <v>1.3787964809940536</v>
+        <v>1.3787964809940543</v>
       </c>
       <c r="J15" t="n" s="307">
-        <v>0.7248976012157514</v>
+        <v>0.7248976012157528</v>
       </c>
     </row>
     <row r="16">
@@ -6363,16 +6363,16 @@
         <v>15.0</v>
       </c>
       <c r="G16" t="n" s="304">
-        <v>0.07795368425375317</v>
+        <v>0.0779536842537526</v>
       </c>
       <c r="H16" t="n" s="305">
-        <v>-1.736774331582869</v>
+        <v>-1.73677433158287</v>
       </c>
       <c r="I16" t="n" s="306">
-        <v>0.07823064004534765</v>
+        <v>0.07823064004534709</v>
       </c>
       <c r="J16" t="n" s="307">
-        <v>-1.7361076610566921</v>
+        <v>-1.7361076610566932</v>
       </c>
     </row>
     <row r="17">
@@ -6395,16 +6395,16 @@
         <v>16.0</v>
       </c>
       <c r="G17" t="n" s="304">
-        <v>1.0207079845622413</v>
+        <v>1.0207079845622404</v>
       </c>
       <c r="H17" t="n" s="305">
-        <v>0.26983677428908237</v>
+        <v>0.26983677428908154</v>
       </c>
       <c r="I17" t="n" s="306">
-        <v>1.119121792241355</v>
+        <v>1.1191217922413546</v>
       </c>
       <c r="J17" t="n" s="307">
-        <v>0.39742266849660457</v>
+        <v>0.3974226684966037</v>
       </c>
     </row>
     <row r="18">
@@ -6427,16 +6427,16 @@
         <v>17.0</v>
       </c>
       <c r="G18" t="n" s="304">
-        <v>0.1759311161090049</v>
+        <v>0.17593111610900497</v>
       </c>
       <c r="H18" t="n" s="305">
-        <v>-1.6808643022018122</v>
+        <v>-1.6808643022018153</v>
       </c>
       <c r="I18" t="n" s="306">
-        <v>0.17066029427481663</v>
+        <v>0.1706602942748168</v>
       </c>
       <c r="J18" t="n" s="307">
-        <v>-1.7351165803715802</v>
+        <v>-1.735116580371582</v>
       </c>
     </row>
     <row r="19">
@@ -6459,16 +6459,16 @@
         <v>18.0</v>
       </c>
       <c r="G19" t="n" s="304">
-        <v>1.0851958570007563</v>
+        <v>1.0851958570007585</v>
       </c>
       <c r="H19" t="n" s="305">
-        <v>0.33801700683908154</v>
+        <v>0.33801700683908487</v>
       </c>
       <c r="I19" t="n" s="306">
-        <v>1.1925776814349007</v>
+        <v>1.1925776814349023</v>
       </c>
       <c r="J19" t="n" s="307">
-        <v>0.5054917883048622</v>
+        <v>0.5054917883048644</v>
       </c>
     </row>
     <row r="20">
@@ -6491,16 +6491,16 @@
         <v>19.0</v>
       </c>
       <c r="G20" t="n" s="304">
-        <v>1.8227575633496595</v>
+        <v>1.8227575633496544</v>
       </c>
       <c r="H20" t="n" s="305">
-        <v>1.1378831054569853</v>
+        <v>1.137883105456982</v>
       </c>
       <c r="I20" t="n" s="306">
-        <v>2.0099453866238024</v>
+        <v>2.0099453866237935</v>
       </c>
       <c r="J20" t="n" s="307">
-        <v>1.3309219551872513</v>
+        <v>1.3309219551872453</v>
       </c>
     </row>
     <row r="21">
@@ -6523,16 +6523,16 @@
         <v>20.0</v>
       </c>
       <c r="G21" t="n" s="304">
-        <v>0.11066303272089646</v>
+        <v>0.1106630327208975</v>
       </c>
       <c r="H21" t="n" s="305">
-        <v>-1.7561266395632482</v>
+        <v>-1.7561266395632396</v>
       </c>
       <c r="I21" t="n" s="306">
-        <v>0.1072388304116706</v>
+        <v>0.10723883041167152</v>
       </c>
       <c r="J21" t="n" s="307">
-        <v>-1.8189380685059042</v>
+        <v>-1.8189380685058962</v>
       </c>
     </row>
     <row r="22">
@@ -6555,16 +6555,16 @@
         <v>21.0</v>
       </c>
       <c r="G22" t="n" s="304">
-        <v>0.025032925133883006</v>
+        <v>0.02503292513388284</v>
       </c>
       <c r="H22" t="n" s="305">
-        <v>-3.470172658130168</v>
+        <v>-3.470172658130172</v>
       </c>
       <c r="I22" t="n" s="306">
-        <v>0.024593291754851563</v>
+        <v>0.024593291754851372</v>
       </c>
       <c r="J22" t="n" s="307">
-        <v>-3.479831632904004</v>
+        <v>-3.4798316329040078</v>
       </c>
     </row>
     <row r="23">
@@ -6587,16 +6587,16 @@
         <v>22.0</v>
       </c>
       <c r="G23" t="n" s="304">
-        <v>0.07795368425375317</v>
+        <v>0.0779536842537526</v>
       </c>
       <c r="H23" t="n" s="305">
-        <v>-1.736774331582869</v>
+        <v>-1.73677433158287</v>
       </c>
       <c r="I23" t="n" s="306">
-        <v>0.07823064004534765</v>
+        <v>0.07823064004534709</v>
       </c>
       <c r="J23" t="n" s="307">
-        <v>-1.7361076610566921</v>
+        <v>-1.7361076610566932</v>
       </c>
     </row>
     <row r="24">
@@ -6619,16 +6619,16 @@
         <v>23.0</v>
       </c>
       <c r="G24" t="n" s="304">
-        <v>0.3834328861064308</v>
+        <v>0.3834328861064314</v>
       </c>
       <c r="H24" t="n" s="305">
-        <v>-0.9586932269411798</v>
+        <v>-0.9586932269411801</v>
       </c>
       <c r="I24" t="n" s="306">
-        <v>0.3878551657926025</v>
+        <v>0.38785516579260304</v>
       </c>
       <c r="J24" t="n" s="307">
-        <v>-0.9658679397707658</v>
+        <v>-0.965867939770766</v>
       </c>
     </row>
     <row r="25">
@@ -6683,16 +6683,16 @@
         <v>25.0</v>
       </c>
       <c r="G26" t="n" s="304">
-        <v>0.6680647268704238</v>
+        <v>0.6680647268704314</v>
       </c>
       <c r="H26" t="n" s="305">
-        <v>-0.13985512847552017</v>
+        <v>-0.1398551284755032</v>
       </c>
       <c r="I26" t="n" s="306">
-        <v>0.61074118070569</v>
+        <v>0.6107411807056929</v>
       </c>
       <c r="J26" t="n" s="307">
-        <v>-0.2503587441086242</v>
+        <v>-0.25035874410861275</v>
       </c>
     </row>
     <row r="27">
@@ -6715,16 +6715,16 @@
         <v>26.0</v>
       </c>
       <c r="G27" t="n" s="304">
-        <v>0.7424757338535903</v>
+        <v>0.742475733853589</v>
       </c>
       <c r="H27" t="n" s="305">
-        <v>-0.211698996397792</v>
+        <v>-0.21169899639779785</v>
       </c>
       <c r="I27" t="n" s="306">
-        <v>0.7305943091963324</v>
+        <v>0.73059430919633</v>
       </c>
       <c r="J27" t="n" s="307">
-        <v>-0.2595729783361783</v>
+        <v>-0.2595729783361863</v>
       </c>
     </row>
     <row r="28">
@@ -6747,16 +6747,16 @@
         <v>27.0</v>
       </c>
       <c r="G28" t="n" s="304">
-        <v>0.07795368425375317</v>
+        <v>0.0779536842537526</v>
       </c>
       <c r="H28" t="n" s="305">
-        <v>-1.736774331582869</v>
+        <v>-1.73677433158287</v>
       </c>
       <c r="I28" t="n" s="306">
-        <v>0.07823064004534765</v>
+        <v>0.07823064004534709</v>
       </c>
       <c r="J28" t="n" s="307">
-        <v>-1.7361076610566921</v>
+        <v>-1.7361076610566932</v>
       </c>
     </row>
     <row r="29">
@@ -6782,13 +6782,13 @@
         <v>5.386977188423378</v>
       </c>
       <c r="H29" t="n" s="305">
-        <v>4.14012635759027</v>
+        <v>4.140126357590274</v>
       </c>
       <c r="I29" t="n" s="306">
-        <v>5.639645274332899</v>
+        <v>5.639645274332895</v>
       </c>
       <c r="J29" t="n" s="307">
-        <v>4.32242217144439</v>
+        <v>4.322422171444389</v>
       </c>
     </row>
     <row r="30">
@@ -6811,16 +6811,16 @@
         <v>29.0</v>
       </c>
       <c r="G30" t="n" s="304">
-        <v>0.4597117512939392</v>
+        <v>0.45971175129394465</v>
       </c>
       <c r="H30" t="n" s="305">
-        <v>-0.28554250315674073</v>
+        <v>-0.2855425031567172</v>
       </c>
       <c r="I30" t="n" s="306">
-        <v>0.4973509656464359</v>
+        <v>0.49735096564644476</v>
       </c>
       <c r="J30" t="n" s="307">
-        <v>-0.24473743580101032</v>
+        <v>-0.2447374358009835</v>
       </c>
     </row>
     <row r="31">
@@ -6843,16 +6843,16 @@
         <v>30.0</v>
       </c>
       <c r="G31" t="n" s="304">
-        <v>0.6897415421153342</v>
+        <v>0.6897415421153362</v>
       </c>
       <c r="H31" t="n" s="305">
-        <v>-0.13420933443717414</v>
+        <v>-0.1342093344371698</v>
       </c>
       <c r="I31" t="n" s="306">
-        <v>0.7200110859282758</v>
+        <v>0.7200110859282782</v>
       </c>
       <c r="J31" t="n" s="307">
-        <v>-0.09547002544099348</v>
+        <v>-0.09547002544098859</v>
       </c>
     </row>
     <row r="32">
@@ -6875,16 +6875,16 @@
         <v>31.0</v>
       </c>
       <c r="G32" t="n" s="304">
-        <v>0.3434986272483214</v>
+        <v>0.3434986272483193</v>
       </c>
       <c r="H32" t="n" s="305">
-        <v>-0.9525118921985917</v>
+        <v>-0.9525118921986003</v>
       </c>
       <c r="I32" t="n" s="306">
-        <v>0.30352077346381684</v>
+        <v>0.303520773463816</v>
       </c>
       <c r="J32" t="n" s="307">
-        <v>-1.1250410322803064</v>
+        <v>-1.125041032280312</v>
       </c>
     </row>
     <row r="33">
@@ -6907,16 +6907,16 @@
         <v>32.0</v>
       </c>
       <c r="G33" t="n" s="304">
-        <v>0.5557137133708635</v>
+        <v>0.5557137133708623</v>
       </c>
       <c r="H33" t="n" s="305">
-        <v>-0.49517666301099694</v>
+        <v>-0.4951766630109993</v>
       </c>
       <c r="I33" t="n" s="306">
-        <v>0.5341783211470723</v>
+        <v>0.5341783211470708</v>
       </c>
       <c r="J33" t="n" s="307">
-        <v>-0.5711799195532402</v>
+        <v>-0.5711799195532433</v>
       </c>
     </row>
     <row r="34">
@@ -6939,16 +6939,16 @@
         <v>33.0</v>
       </c>
       <c r="G34" t="n" s="304">
-        <v>0.035252892800253795</v>
+        <v>0.03525289280025391</v>
       </c>
       <c r="H34" t="n" s="305">
-        <v>-2.1138387284731204</v>
+        <v>-2.113838728473115</v>
       </c>
       <c r="I34" t="n" s="306">
-        <v>0.03660502537171479</v>
+        <v>0.03660502537171496</v>
       </c>
       <c r="J34" t="n" s="307">
-        <v>-2.1263945086237723</v>
+        <v>-2.126394508623765</v>
       </c>
     </row>
     <row r="35">
@@ -6971,16 +6971,16 @@
         <v>34.0</v>
       </c>
       <c r="G35" t="n" s="304">
-        <v>0.8684520546624985</v>
+        <v>0.868452054662498</v>
       </c>
       <c r="H35" t="n" s="305">
-        <v>0.06513822234374081</v>
+        <v>0.06513822234373909</v>
       </c>
       <c r="I35" t="n" s="306">
-        <v>0.8652120048255664</v>
+        <v>0.8652120048255663</v>
       </c>
       <c r="J35" t="n" s="307">
-        <v>0.044085350845146004</v>
+        <v>0.04408535084514528</v>
       </c>
     </row>
     <row r="36">
@@ -7003,16 +7003,16 @@
         <v>35.0</v>
       </c>
       <c r="G36" t="n" s="304">
-        <v>0.5900682597684905</v>
+        <v>0.5900682597684881</v>
       </c>
       <c r="H36" t="n" s="305">
-        <v>-0.5161801413892743</v>
+        <v>-0.5161801413892841</v>
       </c>
       <c r="I36" t="n" s="306">
-        <v>0.6574151133432158</v>
+        <v>0.6574151133432132</v>
       </c>
       <c r="J36" t="n" s="307">
-        <v>-0.40707726470510275</v>
+        <v>-0.40707726470511196</v>
       </c>
     </row>
     <row r="37">
@@ -7035,16 +7035,16 @@
         <v>36.0</v>
       </c>
       <c r="G37" t="n" s="304">
-        <v>1.1460447213585894</v>
+        <v>1.1460447213585865</v>
       </c>
       <c r="H37" t="n" s="305">
-        <v>0.4357788423492477</v>
+        <v>0.435778842349244</v>
       </c>
       <c r="I37" t="n" s="306">
-        <v>1.2050665970086654</v>
+        <v>1.2050665970086638</v>
       </c>
       <c r="J37" t="n" s="307">
-        <v>0.5072756938550897</v>
+        <v>0.507275693855088</v>
       </c>
     </row>
     <row r="38">
@@ -7067,16 +7067,16 @@
         <v>37.0</v>
       </c>
       <c r="G38" t="n" s="304">
-        <v>0.8497888240470558</v>
+        <v>0.8497888240470551</v>
       </c>
       <c r="H38" t="n" s="305">
-        <v>-0.07133772376079658</v>
+        <v>-0.0713377237607987</v>
       </c>
       <c r="I38" t="n" s="306">
-        <v>0.8921955517182776</v>
+        <v>0.8921955517182767</v>
       </c>
       <c r="J38" t="n" s="307">
-        <v>-0.006240375767916473</v>
+        <v>-0.00624037576791836</v>
       </c>
     </row>
     <row r="39">
@@ -7099,16 +7099,16 @@
         <v>38.0</v>
       </c>
       <c r="G39" t="n" s="304">
-        <v>0.9150924430510671</v>
+        <v>0.915092443051069</v>
       </c>
       <c r="H39" t="n" s="305">
-        <v>0.10340919046916683</v>
+        <v>0.10340919046916916</v>
       </c>
       <c r="I39" t="n" s="306">
-        <v>0.9678021771741743</v>
+        <v>0.9678021771741756</v>
       </c>
       <c r="J39" t="n" s="307">
-        <v>0.17915740615870346</v>
+        <v>0.17915740615870507</v>
       </c>
     </row>
     <row r="40">
@@ -7131,16 +7131,16 @@
         <v>39.0</v>
       </c>
       <c r="G40" t="n" s="304">
-        <v>3.8841704989820127</v>
+        <v>3.8841704989820185</v>
       </c>
       <c r="H40" t="n" s="305">
-        <v>2.318300325503491</v>
+        <v>2.3183003255034915</v>
       </c>
       <c r="I40" t="n" s="306">
-        <v>3.92790155975471</v>
+        <v>3.927901559754719</v>
       </c>
       <c r="J40" t="n" s="307">
-        <v>2.357534652742437</v>
+        <v>2.3575346527424372</v>
       </c>
     </row>
     <row r="41">
@@ -7163,16 +7163,16 @@
         <v>40.0</v>
       </c>
       <c r="G41" t="n" s="304">
-        <v>0.6347083541004135</v>
+        <v>0.6347083541004144</v>
       </c>
       <c r="H41" t="n" s="305">
-        <v>-0.3409226303817582</v>
+        <v>-0.34092263038175596</v>
       </c>
       <c r="I41" t="n" s="306">
-        <v>0.6098185115153854</v>
+        <v>0.6098185115153864</v>
       </c>
       <c r="J41" t="n" s="307">
-        <v>-0.41481178204174507</v>
+        <v>-0.41481178204174296</v>
       </c>
     </row>
     <row r="42">
@@ -7195,16 +7195,16 @@
         <v>41.0</v>
       </c>
       <c r="G42" t="n" s="304">
-        <v>0.4601944513377236</v>
+        <v>0.46019445133772274</v>
       </c>
       <c r="H42" t="n" s="305">
-        <v>-0.9608645868722929</v>
+        <v>-0.9608645868722971</v>
       </c>
       <c r="I42" t="n" s="306">
-        <v>0.4712244135398216</v>
+        <v>0.47122441353982064</v>
       </c>
       <c r="J42" t="n" s="307">
-        <v>-0.9770720395356994</v>
+        <v>-0.9770720395357024</v>
       </c>
     </row>
     <row r="43">
@@ -7227,16 +7227,16 @@
         <v>42.0</v>
       </c>
       <c r="G43" t="n" s="304">
-        <v>0.12897246031189663</v>
+        <v>0.12897246031189627</v>
       </c>
       <c r="H43" t="n" s="305">
-        <v>-1.5918316301247635</v>
+        <v>-1.5918316301247626</v>
       </c>
       <c r="I43" t="n" s="306">
-        <v>0.1348532506031248</v>
+        <v>0.13485325060312442</v>
       </c>
       <c r="J43" t="n" s="307">
-        <v>-1.584959081267903</v>
+        <v>-1.5849590812679029</v>
       </c>
     </row>
     <row r="44">
@@ -7259,16 +7259,16 @@
         <v>43.0</v>
       </c>
       <c r="G44" t="n" s="304">
-        <v>1.8503892790174266</v>
+        <v>1.8503892790174228</v>
       </c>
       <c r="H44" t="n" s="305">
-        <v>1.3848735084530037</v>
+        <v>1.3848735084530002</v>
       </c>
       <c r="I44" t="n" s="306">
-        <v>1.8878258935328054</v>
+        <v>1.8878258935328012</v>
       </c>
       <c r="J44" t="n" s="307">
-        <v>1.438956120365507</v>
+        <v>1.4389561203655028</v>
       </c>
     </row>
     <row r="45">
@@ -7291,16 +7291,16 @@
         <v>44.0</v>
       </c>
       <c r="G45" t="n" s="304">
-        <v>0.035252892800253795</v>
+        <v>0.03525289280025391</v>
       </c>
       <c r="H45" t="n" s="305">
-        <v>-2.1138387284731204</v>
+        <v>-2.113838728473115</v>
       </c>
       <c r="I45" t="n" s="306">
-        <v>0.03660502537171479</v>
+        <v>0.03660502537171496</v>
       </c>
       <c r="J45" t="n" s="307">
-        <v>-2.1263945086237723</v>
+        <v>-2.126394508623765</v>
       </c>
     </row>
     <row r="46">
@@ -7323,16 +7323,16 @@
         <v>45.0</v>
       </c>
       <c r="G46" t="n" s="304">
-        <v>0.07974967425702942</v>
+        <v>0.07974967425702918</v>
       </c>
       <c r="H46" t="n" s="305">
-        <v>-2.37847550319841</v>
+        <v>-2.3784755031984264</v>
       </c>
       <c r="I46" t="n" s="306">
-        <v>0.07227735714710204</v>
+        <v>0.07227735714710273</v>
       </c>
       <c r="J46" t="n" s="307">
-        <v>-2.553058239296056</v>
+        <v>-2.5530582392960635</v>
       </c>
     </row>
     <row r="47">
@@ -7355,16 +7355,16 @@
         <v>46.0</v>
       </c>
       <c r="G47" t="n" s="304">
-        <v>0.30467358921308413</v>
+        <v>0.3046735892130851</v>
       </c>
       <c r="H47" t="n" s="305">
-        <v>-0.8301920223333985</v>
+        <v>-0.8301920223333852</v>
       </c>
       <c r="I47" t="n" s="306">
-        <v>0.2770925601892289</v>
+        <v>0.27709256018923184</v>
       </c>
       <c r="J47" t="n" s="307">
-        <v>-0.9428201574983313</v>
+        <v>-0.9428201574983104</v>
       </c>
     </row>
     <row r="48">
@@ -7387,16 +7387,16 @@
         <v>47.0</v>
       </c>
       <c r="G48" t="n" s="304">
-        <v>1.0712831552399382</v>
+        <v>1.0712831552399396</v>
       </c>
       <c r="H48" t="n" s="305">
-        <v>0.35346707416086914</v>
+        <v>0.353467074160871</v>
       </c>
       <c r="I48" t="n" s="306">
-        <v>1.1513422409329401</v>
+        <v>1.1513422409329415</v>
       </c>
       <c r="J48" t="n" s="307">
-        <v>0.4460494026555588</v>
+        <v>0.44604940265555976</v>
       </c>
     </row>
     <row r="49">
@@ -7419,16 +7419,16 @@
         <v>48.0</v>
       </c>
       <c r="G49" t="n" s="304">
-        <v>0.4937087116700346</v>
+        <v>0.4937087116700351</v>
       </c>
       <c r="H49" t="n" s="305">
-        <v>-0.7542008520599918</v>
+        <v>-0.754200852059991</v>
       </c>
       <c r="I49" t="n" s="306">
-        <v>0.4951371375099416</v>
+        <v>0.49513713750994215</v>
       </c>
       <c r="J49" t="n" s="307">
-        <v>-0.7972845789962814</v>
+        <v>-0.79728457899628</v>
       </c>
     </row>
     <row r="50">
@@ -7451,16 +7451,16 @@
         <v>49.0</v>
       </c>
       <c r="G50" t="n" s="304">
-        <v>0.4818048737906991</v>
+        <v>0.48180487379070003</v>
       </c>
       <c r="H50" t="n" s="305">
-        <v>-0.4784546281645396</v>
+        <v>-0.47845462816453665</v>
       </c>
       <c r="I50" t="n" s="306">
-        <v>0.474619229459487</v>
+        <v>0.4746192294594878</v>
       </c>
       <c r="J50" t="n" s="307">
-        <v>-0.49278240982342125</v>
+        <v>-0.49278240982341864</v>
       </c>
     </row>
     <row r="51">
@@ -7483,16 +7483,16 @@
         <v>50.0</v>
       </c>
       <c r="G51" t="n" s="304">
-        <v>1.0310678282342836</v>
+        <v>1.0310678282342827</v>
       </c>
       <c r="H51" t="n" s="305">
-        <v>0.24566880995913837</v>
+        <v>0.2456688099591371</v>
       </c>
       <c r="I51" t="n" s="306">
-        <v>1.0313518076745198</v>
+        <v>1.0313518076745192</v>
       </c>
       <c r="J51" t="n" s="307">
-        <v>0.24480749046949324</v>
+        <v>0.24480749046949196</v>
       </c>
     </row>
     <row r="52">
@@ -7515,16 +7515,16 @@
         <v>51.0</v>
       </c>
       <c r="G52" t="n" s="304">
-        <v>1.9890096709560618</v>
+        <v>1.9890096709560547</v>
       </c>
       <c r="H52" t="n" s="305">
-        <v>1.5418131624891642</v>
+        <v>1.5418131624891573</v>
       </c>
       <c r="I52" t="n" s="306">
-        <v>1.8651749551257237</v>
+        <v>1.8651749551257206</v>
       </c>
       <c r="J52" t="n" s="307">
-        <v>1.4126540733031685</v>
+        <v>1.4126540733031654</v>
       </c>
     </row>
     <row r="53">
@@ -7547,16 +7547,16 @@
         <v>52.0</v>
       </c>
       <c r="G53" t="n" s="304">
-        <v>0.29443234013923514</v>
+        <v>0.2944323401392348</v>
       </c>
       <c r="H53" t="n" s="305">
-        <v>-1.6322986048453416</v>
+        <v>-1.6322986048453438</v>
       </c>
       <c r="I53" t="n" s="306">
-        <v>0.2942052761433762</v>
+        <v>0.29420527614337594</v>
       </c>
       <c r="J53" t="n" s="307">
-        <v>-1.6652070964913854</v>
+        <v>-1.6652070964913885</v>
       </c>
     </row>
     <row r="54">
@@ -7579,16 +7579,16 @@
         <v>53.0</v>
       </c>
       <c r="G54" t="n" s="304">
-        <v>0.01575214441084971</v>
+        <v>0.0157521444108497</v>
       </c>
       <c r="H54" t="n" s="305">
-        <v>-3.7024570228460427</v>
+        <v>-3.7024570228460467</v>
       </c>
       <c r="I54" t="n" s="306">
-        <v>0.016548740608207074</v>
+        <v>0.016548740608207064</v>
       </c>
       <c r="J54" t="n" s="307">
-        <v>-3.720772203211513</v>
+        <v>-3.7207722032115167</v>
       </c>
     </row>
     <row r="55">
@@ -7611,10 +7611,10 @@
         <v>54.0</v>
       </c>
       <c r="G55" t="n" s="304">
-        <v>1.2667847207648784</v>
+        <v>1.2667847207648781</v>
       </c>
       <c r="H55" t="n" s="305">
-        <v>0.5758714162172764</v>
+        <v>0.5758714162172763</v>
       </c>
       <c r="I55" t="n" s="306">
         <v>1.1940647376361413</v>
@@ -7643,16 +7643,16 @@
         <v>55.0</v>
       </c>
       <c r="G56" t="n" s="304">
-        <v>0.525015262862888</v>
+        <v>0.5250152628628876</v>
       </c>
       <c r="H56" t="n" s="305">
-        <v>-0.45959854406358785</v>
+        <v>-0.4595985440635876</v>
       </c>
       <c r="I56" t="n" s="306">
-        <v>0.48637200708491435</v>
+        <v>0.48637200708491357</v>
       </c>
       <c r="J56" t="n" s="307">
-        <v>-0.5467993616561413</v>
+        <v>-0.5467993616561417</v>
       </c>
     </row>
     <row r="57">
@@ -7675,16 +7675,16 @@
         <v>56.0</v>
       </c>
       <c r="G57" t="n" s="304">
-        <v>0.525015262862888</v>
+        <v>0.5250152628628876</v>
       </c>
       <c r="H57" t="n" s="305">
-        <v>-0.45959854406358785</v>
+        <v>-0.4595985440635876</v>
       </c>
       <c r="I57" t="n" s="306">
-        <v>0.48637200708491435</v>
+        <v>0.48637200708491357</v>
       </c>
       <c r="J57" t="n" s="307">
-        <v>-0.5467993616561413</v>
+        <v>-0.5467993616561417</v>
       </c>
     </row>
   </sheetData>
@@ -7770,7 +7770,7 @@
         <v>6.0</v>
       </c>
       <c r="F2" t="n" s="319">
-        <v>1.0</v>
+        <v>10169.0</v>
       </c>
       <c r="G2" t="n" s="320">
         <v>4.0</v>
@@ -7782,13 +7782,13 @@
         <v>28.0</v>
       </c>
       <c r="J2" t="n" s="323">
-        <v>0.8224490761629857</v>
+        <v>0.8224490761629818</v>
       </c>
       <c r="K2" t="n" s="324">
-        <v>0.4844543610234504</v>
+        <v>0.4844543610234488</v>
       </c>
       <c r="L2" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="3">
@@ -7808,7 +7808,7 @@
         <v>4.0</v>
       </c>
       <c r="F3" t="n" s="319">
-        <v>2.0</v>
+        <v>10170.0</v>
       </c>
       <c r="G3" t="n" s="320">
         <v>4.0</v>
@@ -7820,13 +7820,13 @@
         <v>28.0</v>
       </c>
       <c r="J3" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K3" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L3" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="4">
@@ -7846,7 +7846,7 @@
         <v>6.0</v>
       </c>
       <c r="F4" t="n" s="319">
-        <v>3.0</v>
+        <v>10171.0</v>
       </c>
       <c r="G4" t="n" s="320">
         <v>4.0</v>
@@ -7858,13 +7858,13 @@
         <v>28.0</v>
       </c>
       <c r="J4" t="n" s="323">
-        <v>1.2795930062205756</v>
+        <v>1.2795930062205687</v>
       </c>
       <c r="K4" t="n" s="324">
-        <v>0.526949177118505</v>
+        <v>0.5269491771185029</v>
       </c>
       <c r="L4" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="5">
@@ -7884,7 +7884,7 @@
         <v>4.0</v>
       </c>
       <c r="F5" t="n" s="319">
-        <v>4.0</v>
+        <v>10172.0</v>
       </c>
       <c r="G5" t="n" s="320">
         <v>4.0</v>
@@ -7896,13 +7896,13 @@
         <v>28.0</v>
       </c>
       <c r="J5" t="n" s="323">
-        <v>0.6099736974815367</v>
+        <v>0.6099736974815373</v>
       </c>
       <c r="K5" t="n" s="324">
-        <v>0.4794598068941739</v>
+        <v>0.47945980689417467</v>
       </c>
       <c r="L5" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="6">
@@ -7922,7 +7922,7 @@
         <v>6.0</v>
       </c>
       <c r="F6" t="n" s="319">
-        <v>5.0</v>
+        <v>10174.0</v>
       </c>
       <c r="G6" t="n" s="320">
         <v>4.0</v>
@@ -7934,13 +7934,13 @@
         <v>28.0</v>
       </c>
       <c r="J6" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K6" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L6" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="7">
@@ -7960,7 +7960,7 @@
         <v>6.0</v>
       </c>
       <c r="F7" t="n" s="319">
-        <v>6.0</v>
+        <v>10175.0</v>
       </c>
       <c r="G7" t="n" s="320">
         <v>4.0</v>
@@ -7972,13 +7972,13 @@
         <v>28.0</v>
       </c>
       <c r="J7" t="n" s="323">
-        <v>1.2795930062205756</v>
+        <v>1.2795930062205687</v>
       </c>
       <c r="K7" t="n" s="324">
-        <v>0.526949177118505</v>
+        <v>0.5269491771185029</v>
       </c>
       <c r="L7" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="8">
@@ -7998,7 +7998,7 @@
         <v>3.0</v>
       </c>
       <c r="F8" t="n" s="319">
-        <v>7.0</v>
+        <v>10176.0</v>
       </c>
       <c r="G8" t="n" s="320">
         <v>4.0</v>
@@ -8010,13 +8010,13 @@
         <v>28.0</v>
       </c>
       <c r="J8" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K8" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L8" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="9">
@@ -8036,7 +8036,7 @@
         <v>5.0</v>
       </c>
       <c r="F9" t="n" s="319">
-        <v>8.0</v>
+        <v>10178.0</v>
       </c>
       <c r="G9" t="n" s="320">
         <v>4.0</v>
@@ -8048,13 +8048,13 @@
         <v>28.0</v>
       </c>
       <c r="J9" t="n" s="323">
-        <v>0.3948912765942029</v>
+        <v>0.3948912765942006</v>
       </c>
       <c r="K9" t="n" s="324">
         <v>0.48227608647545783</v>
       </c>
       <c r="L9" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="10">
@@ -8074,7 +8074,7 @@
         <v>4.0</v>
       </c>
       <c r="F10" t="n" s="319">
-        <v>9.0</v>
+        <v>10179.0</v>
       </c>
       <c r="G10" t="n" s="320">
         <v>4.0</v>
@@ -8086,13 +8086,13 @@
         <v>28.0</v>
       </c>
       <c r="J10" t="n" s="323">
-        <v>-0.9264124251633018</v>
+        <v>-0.9264124251632988</v>
       </c>
       <c r="K10" t="n" s="324">
         <v>0.48993701124192823</v>
       </c>
       <c r="L10" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="11">
@@ -8112,7 +8112,7 @@
         <v>2.0</v>
       </c>
       <c r="F11" t="n" s="319">
-        <v>10.0</v>
+        <v>10181.0</v>
       </c>
       <c r="G11" t="n" s="320">
         <v>4.0</v>
@@ -8124,13 +8124,13 @@
         <v>28.0</v>
       </c>
       <c r="J11" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K11" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L11" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="12">
@@ -8150,7 +8150,7 @@
         <v>3.0</v>
       </c>
       <c r="F12" t="n" s="319">
-        <v>11.0</v>
+        <v>10183.0</v>
       </c>
       <c r="G12" t="n" s="320">
         <v>4.0</v>
@@ -8162,13 +8162,13 @@
         <v>28.0</v>
       </c>
       <c r="J12" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K12" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L12" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="13">
@@ -8188,7 +8188,7 @@
         <v>4.0</v>
       </c>
       <c r="F13" t="n" s="319">
-        <v>12.0</v>
+        <v>10184.0</v>
       </c>
       <c r="G13" t="n" s="320">
         <v>4.0</v>
@@ -8200,13 +8200,13 @@
         <v>28.0</v>
       </c>
       <c r="J13" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K13" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L13" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="14">
@@ -8226,7 +8226,7 @@
         <v>4.0</v>
       </c>
       <c r="F14" t="n" s="319">
-        <v>13.0</v>
+        <v>10185.0</v>
       </c>
       <c r="G14" t="n" s="320">
         <v>4.0</v>
@@ -8238,13 +8238,13 @@
         <v>28.0</v>
       </c>
       <c r="J14" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K14" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L14" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="15">
@@ -8264,7 +8264,7 @@
         <v>6.0</v>
       </c>
       <c r="F15" t="n" s="319">
-        <v>14.0</v>
+        <v>10186.0</v>
       </c>
       <c r="G15" t="n" s="320">
         <v>4.0</v>
@@ -8276,13 +8276,13 @@
         <v>28.0</v>
       </c>
       <c r="J15" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K15" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L15" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="16">
@@ -8302,7 +8302,7 @@
         <v>4.0</v>
       </c>
       <c r="F16" t="n" s="319">
-        <v>15.0</v>
+        <v>10188.0</v>
       </c>
       <c r="G16" t="n" s="320">
         <v>4.0</v>
@@ -8314,13 +8314,13 @@
         <v>28.0</v>
       </c>
       <c r="J16" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K16" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L16" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="17">
@@ -8340,7 +8340,7 @@
         <v>5.0</v>
       </c>
       <c r="F17" t="n" s="319">
-        <v>16.0</v>
+        <v>10189.0</v>
       </c>
       <c r="G17" t="n" s="320">
         <v>4.0</v>
@@ -8352,13 +8352,13 @@
         <v>28.0</v>
       </c>
       <c r="J17" t="n" s="323">
-        <v>-1.158404210888182</v>
+        <v>-1.1584042108881796</v>
       </c>
       <c r="K17" t="n" s="324">
-        <v>0.46868279509435684</v>
+        <v>0.4686827950943565</v>
       </c>
       <c r="L17" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="18">
@@ -8378,7 +8378,7 @@
         <v>5.0</v>
       </c>
       <c r="F18" t="n" s="319">
-        <v>17.0</v>
+        <v>10190.0</v>
       </c>
       <c r="G18" t="n" s="320">
         <v>4.0</v>
@@ -8390,13 +8390,13 @@
         <v>28.0</v>
       </c>
       <c r="J18" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K18" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L18" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="19">
@@ -8416,7 +8416,7 @@
         <v>7.0</v>
       </c>
       <c r="F19" t="n" s="319">
-        <v>18.0</v>
+        <v>10191.0</v>
       </c>
       <c r="G19" t="n" s="320">
         <v>4.0</v>
@@ -8428,13 +8428,13 @@
         <v>28.0</v>
       </c>
       <c r="J19" t="n" s="323">
-        <v>1.0416617962434764</v>
+        <v>1.041661796243481</v>
       </c>
       <c r="K19" t="n" s="324">
         <v>0.4991231961083929</v>
       </c>
       <c r="L19" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="20">
@@ -8454,7 +8454,7 @@
         <v>7.0</v>
       </c>
       <c r="F20" t="n" s="319">
-        <v>19.0</v>
+        <v>10192.0</v>
       </c>
       <c r="G20" t="n" s="320">
         <v>4.0</v>
@@ -8466,13 +8466,13 @@
         <v>28.0</v>
       </c>
       <c r="J20" t="n" s="323">
-        <v>1.5553167566888355</v>
+        <v>1.5553167566888324</v>
       </c>
       <c r="K20" t="n" s="324">
-        <v>0.5752041012322622</v>
+        <v>0.5752041012322594</v>
       </c>
       <c r="L20" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="21">
@@ -8492,7 +8492,7 @@
         <v>4.0</v>
       </c>
       <c r="F21" t="n" s="319">
-        <v>20.0</v>
+        <v>10193.0</v>
       </c>
       <c r="G21" t="n" s="320">
         <v>4.0</v>
@@ -8504,13 +8504,13 @@
         <v>28.0</v>
       </c>
       <c r="J21" t="n" s="323">
-        <v>-0.08038848747269554</v>
+        <v>-0.08038848747269549</v>
       </c>
       <c r="K21" t="n" s="324">
-        <v>0.5043580861250043</v>
+        <v>0.5043580861250034</v>
       </c>
       <c r="L21" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="22">
@@ -8530,7 +8530,7 @@
         <v>5.0</v>
       </c>
       <c r="F22" t="n" s="319">
-        <v>21.0</v>
+        <v>10195.0</v>
       </c>
       <c r="G22" t="n" s="320">
         <v>4.0</v>
@@ -8542,13 +8542,13 @@
         <v>28.0</v>
       </c>
       <c r="J22" t="n" s="323">
-        <v>0.6099736974815367</v>
+        <v>0.6099736974815373</v>
       </c>
       <c r="K22" t="n" s="324">
-        <v>0.4794598068941739</v>
+        <v>0.47945980689417467</v>
       </c>
       <c r="L22" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="23">
@@ -8568,7 +8568,7 @@
         <v>4.0</v>
       </c>
       <c r="F23" t="n" s="319">
-        <v>22.0</v>
+        <v>10196.0</v>
       </c>
       <c r="G23" t="n" s="320">
         <v>4.0</v>
@@ -8580,13 +8580,13 @@
         <v>28.0</v>
       </c>
       <c r="J23" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K23" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L23" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="24">
@@ -8606,7 +8606,7 @@
         <v>5.0</v>
       </c>
       <c r="F24" t="n" s="319">
-        <v>23.0</v>
+        <v>10197.0</v>
       </c>
       <c r="G24" t="n" s="320">
         <v>4.0</v>
@@ -8618,13 +8618,13 @@
         <v>28.0</v>
       </c>
       <c r="J24" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K24" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L24" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="25">
@@ -8644,7 +8644,7 @@
         <v>1.0</v>
       </c>
       <c r="F25" t="n" s="319">
-        <v>24.0</v>
+        <v>10199.0</v>
       </c>
       <c r="G25" t="n" s="320">
         <v>4.0</v>
@@ -8656,13 +8656,13 @@
         <v>28.0</v>
       </c>
       <c r="J25" t="n" s="323">
-        <v>-1.3607329886887969</v>
+        <v>-1.3607329886887949</v>
       </c>
       <c r="K25" t="n" s="324">
-        <v>0.45264088727971835</v>
+        <v>0.45264088727971863</v>
       </c>
       <c r="L25" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="26">
@@ -8682,7 +8682,7 @@
         <v>7.0</v>
       </c>
       <c r="F26" t="n" s="319">
-        <v>25.0</v>
+        <v>10200.0</v>
       </c>
       <c r="G26" t="n" s="320">
         <v>4.0</v>
@@ -8694,13 +8694,13 @@
         <v>28.0</v>
       </c>
       <c r="J26" t="n" s="323">
-        <v>1.906540406011503</v>
+        <v>1.9065404060115256</v>
       </c>
       <c r="K26" t="n" s="324">
-        <v>0.661225755407761</v>
+        <v>0.6612257554077733</v>
       </c>
       <c r="L26" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="27">
@@ -8720,7 +8720,7 @@
         <v>5.0</v>
       </c>
       <c r="F27" t="n" s="319">
-        <v>26.0</v>
+        <v>10201.0</v>
       </c>
       <c r="G27" t="n" s="320">
         <v>4.0</v>
@@ -8732,13 +8732,13 @@
         <v>28.0</v>
       </c>
       <c r="J27" t="n" s="323">
-        <v>1.2795930062205756</v>
+        <v>1.2795930062205687</v>
       </c>
       <c r="K27" t="n" s="324">
-        <v>0.526949177118505</v>
+        <v>0.5269491771185029</v>
       </c>
       <c r="L27" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="28">
@@ -8758,7 +8758,7 @@
         <v>4.0</v>
       </c>
       <c r="F28" t="n" s="319">
-        <v>27.0</v>
+        <v>10202.0</v>
       </c>
       <c r="G28" t="n" s="320">
         <v>4.0</v>
@@ -8770,13 +8770,13 @@
         <v>28.0</v>
       </c>
       <c r="J28" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K28" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L28" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="29">
@@ -8796,7 +8796,7 @@
         <v>1.0</v>
       </c>
       <c r="F29" t="n" s="319">
-        <v>28.0</v>
+        <v>10203.0</v>
       </c>
       <c r="G29" t="n" s="320">
         <v>4.0</v>
@@ -8808,13 +8808,13 @@
         <v>28.0</v>
       </c>
       <c r="J29" t="n" s="323">
-        <v>0.8224490761629857</v>
+        <v>0.8224490761629818</v>
       </c>
       <c r="K29" t="n" s="324">
-        <v>0.4844543610234504</v>
+        <v>0.4844543610234488</v>
       </c>
       <c r="L29" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="30">
@@ -8834,7 +8834,7 @@
         <v>7.0</v>
       </c>
       <c r="F30" t="n" s="319">
-        <v>29.0</v>
+        <v>10204.0</v>
       </c>
       <c r="G30" t="n" s="320">
         <v>4.0</v>
@@ -8846,13 +8846,13 @@
         <v>28.0</v>
       </c>
       <c r="J30" t="n" s="323">
-        <v>2.4308781157102293</v>
+        <v>2.4308781157102737</v>
       </c>
       <c r="K30" t="n" s="324">
-        <v>0.8388341444082001</v>
+        <v>0.8388341444082169</v>
       </c>
       <c r="L30" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="31">
@@ -8872,7 +8872,7 @@
         <v>3.0</v>
       </c>
       <c r="F31" t="n" s="319">
-        <v>30.0</v>
+        <v>10206.0</v>
       </c>
       <c r="G31" t="n" s="320">
         <v>4.0</v>
@@ -8884,13 +8884,13 @@
         <v>28.0</v>
       </c>
       <c r="J31" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K31" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L31" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="32">
@@ -8910,7 +8910,7 @@
         <v>6.0</v>
       </c>
       <c r="F32" t="n" s="319">
-        <v>31.0</v>
+        <v>10208.0</v>
       </c>
       <c r="G32" t="n" s="320">
         <v>4.0</v>
@@ -8922,13 +8922,13 @@
         <v>28.0</v>
       </c>
       <c r="J32" t="n" s="323">
-        <v>1.5553167566888355</v>
+        <v>1.5553167566888324</v>
       </c>
       <c r="K32" t="n" s="324">
-        <v>0.5752041012322622</v>
+        <v>0.5752041012322594</v>
       </c>
       <c r="L32" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="33">
@@ -8948,7 +8948,7 @@
         <v>4.0</v>
       </c>
       <c r="F33" t="n" s="319">
-        <v>32.0</v>
+        <v>10209.0</v>
       </c>
       <c r="G33" t="n" s="320">
         <v>4.0</v>
@@ -8960,13 +8960,13 @@
         <v>28.0</v>
       </c>
       <c r="J33" t="n" s="323">
-        <v>-1.158404210888182</v>
+        <v>-1.1584042108881796</v>
       </c>
       <c r="K33" t="n" s="324">
-        <v>0.46868279509435684</v>
+        <v>0.4686827950943565</v>
       </c>
       <c r="L33" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="34">
@@ -8986,7 +8986,7 @@
         <v>4.0</v>
       </c>
       <c r="F34" t="n" s="319">
-        <v>33.0</v>
+        <v>10210.0</v>
       </c>
       <c r="G34" t="n" s="320">
         <v>4.0</v>
@@ -8998,13 +8998,13 @@
         <v>28.0</v>
       </c>
       <c r="J34" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K34" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L34" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="35">
@@ -9024,7 +9024,7 @@
         <v>6.0</v>
       </c>
       <c r="F35" t="n" s="319">
-        <v>34.0</v>
+        <v>10211.0</v>
       </c>
       <c r="G35" t="n" s="320">
         <v>4.0</v>
@@ -9036,13 +9036,13 @@
         <v>28.0</v>
       </c>
       <c r="J35" t="n" s="323">
-        <v>1.5553167566888355</v>
+        <v>1.5553167566888324</v>
       </c>
       <c r="K35" t="n" s="324">
-        <v>0.5752041012322622</v>
+        <v>0.5752041012322594</v>
       </c>
       <c r="L35" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="36">
@@ -9062,7 +9062,7 @@
         <v>7.0</v>
       </c>
       <c r="F36" t="n" s="319">
-        <v>35.0</v>
+        <v>10212.0</v>
       </c>
       <c r="G36" t="n" s="320">
         <v>4.0</v>
@@ -9074,13 +9074,13 @@
         <v>28.0</v>
       </c>
       <c r="J36" t="n" s="323">
-        <v>1.2795930062205756</v>
+        <v>1.2795930062205687</v>
       </c>
       <c r="K36" t="n" s="324">
-        <v>0.526949177118505</v>
+        <v>0.5269491771185029</v>
       </c>
       <c r="L36" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="37">
@@ -9100,7 +9100,7 @@
         <v>7.0</v>
       </c>
       <c r="F37" t="n" s="319">
-        <v>36.0</v>
+        <v>10213.0</v>
       </c>
       <c r="G37" t="n" s="320">
         <v>4.0</v>
@@ -9112,13 +9112,13 @@
         <v>28.0</v>
       </c>
       <c r="J37" t="n" s="323">
-        <v>1.5553167566888355</v>
+        <v>1.5553167566888324</v>
       </c>
       <c r="K37" t="n" s="324">
-        <v>0.5752041012322622</v>
+        <v>0.5752041012322594</v>
       </c>
       <c r="L37" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="38">
@@ -9138,7 +9138,7 @@
         <v>1.0</v>
       </c>
       <c r="F38" t="n" s="319">
-        <v>37.0</v>
+        <v>10214.0</v>
       </c>
       <c r="G38" t="n" s="320">
         <v>4.0</v>
@@ -9150,13 +9150,13 @@
         <v>28.0</v>
       </c>
       <c r="J38" t="n" s="323">
-        <v>-1.5460174618832239</v>
+        <v>-1.546017461883222</v>
       </c>
       <c r="K38" t="n" s="324">
-        <v>0.4434453204926454</v>
+        <v>0.4434453204926457</v>
       </c>
       <c r="L38" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="39">
@@ -9176,7 +9176,7 @@
         <v>4.0</v>
       </c>
       <c r="F39" t="n" s="319">
-        <v>38.0</v>
+        <v>10215.0</v>
       </c>
       <c r="G39" t="n" s="320">
         <v>4.0</v>
@@ -9188,13 +9188,13 @@
         <v>28.0</v>
       </c>
       <c r="J39" t="n" s="323">
-        <v>0.1681393885805337</v>
+        <v>0.16813938858053856</v>
       </c>
       <c r="K39" t="n" s="324">
         <v>0.4914511555030068</v>
       </c>
       <c r="L39" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="40">
@@ -9214,7 +9214,7 @@
         <v>1.0</v>
       </c>
       <c r="F40" t="n" s="319">
-        <v>39.0</v>
+        <v>10216.0</v>
       </c>
       <c r="G40" t="n" s="320">
         <v>4.0</v>
@@ -9226,13 +9226,13 @@
         <v>28.0</v>
       </c>
       <c r="J40" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K40" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L40" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="41">
@@ -9252,7 +9252,7 @@
         <v>2.0</v>
       </c>
       <c r="F41" t="n" s="319">
-        <v>40.0</v>
+        <v>10217.0</v>
       </c>
       <c r="G41" t="n" s="320">
         <v>4.0</v>
@@ -9264,13 +9264,13 @@
         <v>28.0</v>
       </c>
       <c r="J41" t="n" s="323">
-        <v>-1.158404210888182</v>
+        <v>-1.1584042108881796</v>
       </c>
       <c r="K41" t="n" s="324">
-        <v>0.46868279509435684</v>
+        <v>0.4686827950943565</v>
       </c>
       <c r="L41" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="42">
@@ -9290,7 +9290,7 @@
         <v>2.0</v>
       </c>
       <c r="F42" t="n" s="319">
-        <v>41.0</v>
+        <v>10218.0</v>
       </c>
       <c r="G42" t="n" s="320">
         <v>4.0</v>
@@ -9302,13 +9302,13 @@
         <v>28.0</v>
       </c>
       <c r="J42" t="n" s="323">
-        <v>-1.5460174618832239</v>
+        <v>-1.546017461883222</v>
       </c>
       <c r="K42" t="n" s="324">
-        <v>0.4434453204926454</v>
+        <v>0.4434453204926457</v>
       </c>
       <c r="L42" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="43">
@@ -9328,7 +9328,7 @@
         <v>3.0</v>
       </c>
       <c r="F43" t="n" s="319">
-        <v>42.0</v>
+        <v>10219.0</v>
       </c>
       <c r="G43" t="n" s="320">
         <v>4.0</v>
@@ -9340,13 +9340,13 @@
         <v>28.0</v>
       </c>
       <c r="J43" t="n" s="323">
-        <v>-0.9264124251633018</v>
+        <v>-0.9264124251632988</v>
       </c>
       <c r="K43" t="n" s="324">
         <v>0.48993701124192823</v>
       </c>
       <c r="L43" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="44">
@@ -9366,7 +9366,7 @@
         <v>7.0</v>
       </c>
       <c r="F44" t="n" s="319">
-        <v>43.0</v>
+        <v>10220.0</v>
       </c>
       <c r="G44" t="n" s="320">
         <v>4.0</v>
@@ -9378,13 +9378,13 @@
         <v>28.0</v>
       </c>
       <c r="J44" t="n" s="323">
-        <v>0.8224490761629857</v>
+        <v>0.8224490761629818</v>
       </c>
       <c r="K44" t="n" s="324">
-        <v>0.4844543610234504</v>
+        <v>0.4844543610234488</v>
       </c>
       <c r="L44" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="45">
@@ -9404,7 +9404,7 @@
         <v>4.0</v>
       </c>
       <c r="F45" t="n" s="319">
-        <v>44.0</v>
+        <v>10221.0</v>
       </c>
       <c r="G45" t="n" s="320">
         <v>4.0</v>
@@ -9416,13 +9416,13 @@
         <v>28.0</v>
       </c>
       <c r="J45" t="n" s="323">
-        <v>-0.3588140158678737</v>
+        <v>-0.3588140158678762</v>
       </c>
       <c r="K45" t="n" s="324">
         <v>0.5140925201529228</v>
       </c>
       <c r="L45" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="46">
@@ -9442,7 +9442,7 @@
         <v>6.0</v>
       </c>
       <c r="F46" t="n" s="319">
-        <v>45.0</v>
+        <v>10223.0</v>
       </c>
       <c r="G46" t="n" s="320">
         <v>4.0</v>
@@ -9454,13 +9454,13 @@
         <v>28.0</v>
       </c>
       <c r="J46" t="n" s="323">
-        <v>1.2795930062205756</v>
+        <v>1.2795930062205687</v>
       </c>
       <c r="K46" t="n" s="324">
-        <v>0.526949177118505</v>
+        <v>0.5269491771185029</v>
       </c>
       <c r="L46" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="47">
@@ -9480,7 +9480,7 @@
         <v>6.0</v>
       </c>
       <c r="F47" t="n" s="319">
-        <v>46.0</v>
+        <v>10224.0</v>
       </c>
       <c r="G47" t="n" s="320">
         <v>4.0</v>
@@ -9492,13 +9492,13 @@
         <v>28.0</v>
       </c>
       <c r="J47" t="n" s="323">
-        <v>1.906540406011503</v>
+        <v>1.9065404060115256</v>
       </c>
       <c r="K47" t="n" s="324">
-        <v>0.661225755407761</v>
+        <v>0.6612257554077733</v>
       </c>
       <c r="L47" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="48">
@@ -9518,7 +9518,7 @@
         <v>5.0</v>
       </c>
       <c r="F48" t="n" s="319">
-        <v>47.0</v>
+        <v>10226.0</v>
       </c>
       <c r="G48" t="n" s="320">
         <v>4.0</v>
@@ -9530,13 +9530,13 @@
         <v>28.0</v>
       </c>
       <c r="J48" t="n" s="323">
-        <v>-0.9264124251633018</v>
+        <v>-0.9264124251632988</v>
       </c>
       <c r="K48" t="n" s="324">
         <v>0.48993701124192823</v>
       </c>
       <c r="L48" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="49">
@@ -9556,7 +9556,7 @@
         <v>2.0</v>
       </c>
       <c r="F49" t="n" s="319">
-        <v>48.0</v>
+        <v>10227.0</v>
       </c>
       <c r="G49" t="n" s="320">
         <v>4.0</v>
@@ -9568,13 +9568,13 @@
         <v>28.0</v>
       </c>
       <c r="J49" t="n" s="323">
-        <v>-2.2869607225549755</v>
+        <v>-2.2869607225549737</v>
       </c>
       <c r="K49" t="n" s="324">
-        <v>0.4845878947286735</v>
+        <v>0.48458789472867325</v>
       </c>
       <c r="L49" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="50">
@@ -9594,7 +9594,7 @@
         <v>3.0</v>
       </c>
       <c r="F50" t="n" s="319">
-        <v>49.0</v>
+        <v>10228.0</v>
       </c>
       <c r="G50" t="n" s="320">
         <v>4.0</v>
@@ -9606,13 +9606,13 @@
         <v>28.0</v>
       </c>
       <c r="J50" t="n" s="323">
-        <v>-0.6543326517017437</v>
+        <v>-0.6543326517017418</v>
       </c>
       <c r="K50" t="n" s="324">
         <v>0.5092799511321389</v>
       </c>
       <c r="L50" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="51">
@@ -9632,7 +9632,7 @@
         <v>3.0</v>
       </c>
       <c r="F51" t="n" s="319">
-        <v>50.0</v>
+        <v>10230.0</v>
       </c>
       <c r="G51" t="n" s="320">
         <v>4.0</v>
@@ -9644,13 +9644,13 @@
         <v>28.0</v>
       </c>
       <c r="J51" t="n" s="323">
-        <v>-2.086394508424926</v>
+        <v>-2.086394508424924</v>
       </c>
       <c r="K51" t="n" s="324">
-        <v>0.46002047589255113</v>
+        <v>0.4600204758925513</v>
       </c>
       <c r="L51" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="52">
@@ -9670,7 +9670,7 @@
         <v>7.0</v>
       </c>
       <c r="F52" t="n" s="319">
-        <v>51.0</v>
+        <v>10232.0</v>
       </c>
       <c r="G52" t="n" s="320">
         <v>4.0</v>
@@ -9682,13 +9682,13 @@
         <v>28.0</v>
       </c>
       <c r="J52" t="n" s="323">
-        <v>0.8224490761629857</v>
+        <v>0.8224490761629818</v>
       </c>
       <c r="K52" t="n" s="324">
-        <v>0.4844543610234504</v>
+        <v>0.4844543610234488</v>
       </c>
       <c r="L52" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="53">
@@ -9708,7 +9708,7 @@
         <v>3.0</v>
       </c>
       <c r="F53" t="n" s="319">
-        <v>52.0</v>
+        <v>10233.0</v>
       </c>
       <c r="G53" t="n" s="320">
         <v>4.0</v>
@@ -9720,13 +9720,13 @@
         <v>28.0</v>
       </c>
       <c r="J53" t="n" s="323">
-        <v>-1.7237587284917097</v>
+        <v>-1.723758728491708</v>
       </c>
       <c r="K53" t="n" s="324">
-        <v>0.4412765460507779</v>
+        <v>0.4412765460507783</v>
       </c>
       <c r="L53" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="54">
@@ -9746,7 +9746,7 @@
         <v>2.0</v>
       </c>
       <c r="F54" t="n" s="319">
-        <v>53.0</v>
+        <v>10234.0</v>
       </c>
       <c r="G54" t="n" s="320">
         <v>4.0</v>
@@ -9758,13 +9758,13 @@
         <v>28.0</v>
       </c>
       <c r="J54" t="n" s="323">
-        <v>-2.086394508424926</v>
+        <v>-2.086394508424924</v>
       </c>
       <c r="K54" t="n" s="324">
-        <v>0.46002047589255113</v>
+        <v>0.4600204758925513</v>
       </c>
       <c r="L54" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="55">
@@ -9784,7 +9784,7 @@
         <v>3.0</v>
       </c>
       <c r="F55" t="n" s="319">
-        <v>54.0</v>
+        <v>10237.0</v>
       </c>
       <c r="G55" t="n" s="320">
         <v>4.0</v>
@@ -9796,13 +9796,13 @@
         <v>28.0</v>
       </c>
       <c r="J55" t="n" s="323">
-        <v>-0.08038848747269554</v>
+        <v>-0.08038848747269549</v>
       </c>
       <c r="K55" t="n" s="324">
-        <v>0.5043580861250043</v>
+        <v>0.5043580861250034</v>
       </c>
       <c r="L55" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="56">
@@ -9822,7 +9822,7 @@
         <v>4.0</v>
       </c>
       <c r="F56" t="n" s="319">
-        <v>55.0</v>
+        <v>10238.0</v>
       </c>
       <c r="G56" t="n" s="320">
         <v>4.0</v>
@@ -9834,13 +9834,13 @@
         <v>28.0</v>
       </c>
       <c r="J56" t="n" s="323">
-        <v>-0.9264124251633018</v>
+        <v>-0.9264124251632988</v>
       </c>
       <c r="K56" t="n" s="324">
         <v>0.48993701124192823</v>
       </c>
       <c r="L56" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
     <row r="57">
@@ -9860,7 +9860,7 @@
         <v>4.0</v>
       </c>
       <c r="F57" t="n" s="319">
-        <v>56.0</v>
+        <v>10240.0</v>
       </c>
       <c r="G57" t="n" s="320">
         <v>4.0</v>
@@ -9872,13 +9872,13 @@
         <v>28.0</v>
       </c>
       <c r="J57" t="n" s="323">
-        <v>-0.9264124251633018</v>
+        <v>-0.9264124251632988</v>
       </c>
       <c r="K57" t="n" s="324">
         <v>0.48993701124192823</v>
       </c>
       <c r="L57" t="n" s="325">
-        <v>0.7953280307097808</v>
+        <v>0.7953280307097809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>